<commit_message>
Tidy up and branding
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jules\Documents\Development Areas\CBS Workflow\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A74D15D-B2AF-4F03-AA50-B6BD9BFF71FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E57DF236-0DB8-461E-93B3-B61DD7A27AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <definedName name="temp">'[1]Station Data'!#REF!</definedName>
     <definedName name="Week">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 

</xml_diff>

<commit_message>
Adding basic workflow functionality
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jules\Documents\Development Areas\CBS Workflow\Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E57DF236-0DB8-461E-93B3-B61DD7A27AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68E8EC75-9709-4676-B36E-997D87E2F976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
First step of GUI
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68E8EC75-9709-4676-B36E-997D87E2F976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F0279AE-37F0-4599-9A98-0A41C73618D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -60,7 +60,19 @@
     <definedName name="temp">'[1]Station Data'!#REF!</definedName>
     <definedName name="Week">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -121,6 +133,4850 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1514" name="Main Screen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{994268F4-613B-3A45-6406-369B73DE290C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="23177500" cy="25400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="1B998B"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="1B998B"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1516" name="MenuBar">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1417B528-A957-BD8F-6B6F-A5DD43616155}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1968500" cy="25400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1515" name="Rectangle 1514" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B350D404-E2C6-99CF-596B-C059F5B75502}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="127000" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1517" name="MenuItem - For Action">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C64942C1-8977-328B-E0B6-20CB2CD21611}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1905000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="476C9B"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="28E5D0"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>For Action</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1518" name="MenuItem - Active">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1029868-E22C-6069-E3A0-2AD4F1526504}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2286000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="476C9B"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="28E5D0"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Active</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1519" name="MenuItem - Complete">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D33D3FC-80AA-4CFD-09CC-F85AF7A75879}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2667000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="476C9B"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="28E5D0"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Complete</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1520" name="MenuItem - Dashboard">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6910506D-6172-D2A5-3790-81226C564758}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="476C9B"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="28E5D0"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Dashboard</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1521" name="MenuItem - Reports">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{116043B4-9EB3-E423-10D1-E640DCABA4FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3429000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="476C9B"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="28E5D0"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Reports</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(6)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1522" name="MenuItem - Admin">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{815D582E-5CC4-E2D4-450A-F874746DF8E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3810000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="476C9B"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="28E5D0"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Admin</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(7)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1523" name="MenuItem - Exit">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB24394-3CC0-B46A-3764-D18E512B7E96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4191000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="3D4547"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="476C9B"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="28E5D0"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Exit</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1525" name="Main Frame">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCDD66AE-D911-A403-211B-018796F22AC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="889000"/>
+          <a:ext cx="11303000" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1524" name="Main Frame Header">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0217C7C2-553B-2059-EA09-DF6A28246F3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="889000"/>
+          <a:ext cx="11303000" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="06BEBD"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="06BEBD"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Active CDC Workflows</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Name&quot;), &quot;UIActive&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1527" name="TextBox 1526">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D5C72C2-E05C-6471-A2FB-D0B45837AB4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1155700"/>
+          <a:ext cx="1524000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;SSN&quot;), &quot;UIActive&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1528" name="TextBox 1527">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BC27FC8-FFBE-8470-DD02-8CBCA92AEC9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3683000" y="1155700"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SSN</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Student ID&quot;), &quot;UIActive&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1529" name="TextBox 1528">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16BC199A-9172-DE6A-CF8A-5AAEB8E3BB7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4699000" y="1155700"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Student ID</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Watch&quot;), &quot;UIActive&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1530" name="TextBox 1529">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21AE62F9-C758-BFA1-5392-E4260C9CC6FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="1155700"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Watch</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;DoD Certification&quot;), &quot;UIActive&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1531" name="TextBox 1530">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22DD6231-0F04-77F5-0806-75AA2A9C6141}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="1155700"/>
+          <a:ext cx="1905000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>DoD Certification</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step No&quot;), &quot;UIActive&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1532" name="TextBox 1531">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B32E0B4-6595-3B4B-D481-F3D27A363BF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="1155700"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Step No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step Name&quot;), &quot;UIActive&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1533" name="TextBox 1532">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{810DD8A4-62E8-CA89-3794-1E4C9DFCE797}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="1155700"/>
+          <a:ext cx="3048000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Step Name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Status&quot;), &quot;UIActive&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1534" name="TextBox 1533">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFB14E80-C57D-663B-9DD4-8DFBD42292DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1155700"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Status</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1535" name="TextBox 1534">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A3ED9FA-DAF4-550A-DBBC-28A7EEB842DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1422400"/>
+          <a:ext cx="1524000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1536" name="TextBox 1535">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{343027B6-B361-018B-02CE-2AF4707D80AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3683000" y="1422400"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1537" name="TextBox 1536">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F229A3-A211-24FA-04F7-5E14B5B15269}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4699000" y="1422400"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1538" name="TextBox 1537">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D35BF053-6B68-4A26-922D-22480A83010C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="1422400"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1539" name="TextBox 1538">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD6EB310-535C-D6CA-4CB5-CF047245746D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="1422400"/>
+          <a:ext cx="1905000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1540" name="TextBox 1539">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F8AD0BF-B2F7-2312-C14F-D3B9CD88D370}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="1422400"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="476C9B"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.03</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1541" name="TextBox 1540">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D27B96F2-CAC1-DBDE-69F8-960D7DA6667C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="1422400"/>
+          <a:ext cx="3048000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="476C9B"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Complete enrolment</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1542" name="TextBox 1541">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38FD1B40-FCBC-9C40-86AD-B3E5FE7E7A93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1422400"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3EC300"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="4AEE00"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Waiting</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1543" name="TextBox 1542">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FFFD19-F5F6-D76C-B591-DFF8323E6F04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1689100"/>
+          <a:ext cx="1524000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1544" name="TextBox 1543">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2779E98B-FA91-192F-5DCA-5FE41D64A715}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3683000" y="1689100"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1545" name="TextBox 1544">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AAE1F6E-C524-3CB3-B4A0-ED71F29FE8DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4699000" y="1689100"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1546" name="TextBox 1545">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FF18509-98D5-5625-0319-61C2AE1BB6B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="1689100"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1547" name="TextBox 1546">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{037E8F38-4C7E-EE04-ED63-221DEF049494}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="1689100"/>
+          <a:ext cx="1905000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1548" name="TextBox 1547">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07CF6CC9-56A1-0AB8-6C23-72800105521E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="1689100"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="476C9B"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.01</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1549" name="TextBox 1548">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D82CDEF1-F3AA-761A-EEED-9132FA4338F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="1689100"/>
+          <a:ext cx="3048000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="476C9B"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Enter Enrollment Date</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1550" name="TextBox 1549">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE75B321-9017-4032-177B-41A0F963D3F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1689100"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3EC300"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="4AEE00"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Action Req'd</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1551" name="TextBox 1550">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B746ADF-2FD7-D9D6-CE89-CA43F4D690BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1955800"/>
+          <a:ext cx="1524000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1552" name="TextBox 1551">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6A2FB64-E5CB-FD33-6672-20F7DD389875}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3683000" y="1955800"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1553" name="TextBox 1552">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33EDB7BB-9FA9-1BD8-7FDE-BF80FE61B7FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4699000" y="1955800"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1554" name="TextBox 1553">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4FFD4F2-29E5-FF1B-72D5-74DBA875C770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="1955800"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1555" name="TextBox 1554">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A58D70D4-6328-809B-B445-6AF2E1314E09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="1955800"/>
+          <a:ext cx="1905000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1556" name="TextBox 1555">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64DCA613-0284-EA26-5A3C-5AB6066420F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="1955800"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="476C9B"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.03</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1557" name="TextBox 1556">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63224058-C26C-202B-1D41-58EEEFF07ADD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="1955800"/>
+          <a:ext cx="3048000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="476C9B"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Complete enrolment</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1558" name="TextBox 1557">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D769F8B5-05D1-18EB-04F5-93B4479136DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1955800"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3EC300"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="4AEE00"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Waiting</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1559" name="TextBox 1558">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F5E5455-DA50-56AC-1216-B87755C9E587}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="2222500"/>
+          <a:ext cx="1524000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1560" name="TextBox 1559">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{244B7BC0-1DE0-ED96-C3BB-9A03DCC63347}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3683000" y="2222500"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1561" name="TextBox 1560">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D31F3F0B-30FA-01DD-913C-257580E6ECBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4699000" y="2222500"/>
+          <a:ext cx="1016000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1562" name="TextBox 1561">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31AE5343-C185-727E-691A-B243ED243651}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="2222500"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1563" name="TextBox 1562">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F428C74D-73E5-2CD7-92D8-8A7899A62226}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="2222500"/>
+          <a:ext cx="1905000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="476C9B"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1564" name="TextBox 1563">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A8ADDA-5D86-EBF2-4F78-6E0BF9621A9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="2222500"/>
+          <a:ext cx="762000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="476C9B"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.01</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1565" name="TextBox 1564">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31E315F1-FCE1-2BE8-C326-914D569605AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="2222500"/>
+          <a:ext cx="3048000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F6F7EB"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="476C9B"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Enter Enrollment Date</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIActive.OpenWorkflow(5)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1566" name="TextBox 1565">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DE1CB8D-6E6D-44FC-40B6-D9BB0777D8FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="2222500"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3EC300"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="4AEE00"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Action Req'd</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.ProcessBtnPress(6)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1526" name="BtnMain1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{542C79EE-641F-DA80-6015-697312523CD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="190500"/>
+          <a:ext cx="1270000" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="06BEBD"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="28E5D0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="3D4547"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>New Workflow</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1567" name="Rectangle 1566">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0752C6B1-9F79-FFC8-73B2-93AC5710A9F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="127000" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1568" name="Main Frame">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{554D7846-9012-86AC-E1E6-FE870C06EE83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="127000" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6190,13 +11046,17 @@
   <dimension ref="A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Class conversion away from pointers
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BABE81B-3CA1-4A39-8B88-9AE750C8A67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0521A4CF-1B17-4A72-ACF1-9D9E008FE167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7725" yWindow="1485" windowWidth="30615" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18405" yWindow="2370" windowWidth="21870" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -101,6 +101,98 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Main Screen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65EABD0C-F5D3-DFF9-C92D-103E86CBDA59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="23177500" cy="25400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FBF9FF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FBF9FF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>39</xdr:col>
@@ -149,6 +241,1819 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{450591C2-4C83-D31D-951F-7E9D573655E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="127000" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="MenuBar">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D428F533-7224-E8FA-B279-2EC0860F95BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1968500" cy="25400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:prstClr val="black"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A4C97E-42C2-8EB1-8A68-C8B2D4E84FFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="127000" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127001</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47488</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>165101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{641AA52D-312B-5460-CE5A-C71560E530F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="127001" y="165101"/>
+          <a:ext cx="1749287" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="MenuItem - For Action">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AADA3A66-9E7B-5352-44C6-706E26F93ED0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1905000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="D8336B"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="D8336B"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="134F69"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>For Action</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="MenuItem - Active">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57DF0E0F-6539-8104-42A5-A21BE67D0D8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2286000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="134F69"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Active</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(3)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="MenuItem - Complete">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDF0BED-0652-E878-FABC-B6D9A06075EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2667000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="134F69"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Complete</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(4)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="MenuItem - Exit">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0886AC73-2D5E-A581-412A-D68455787488}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="134F69"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Exit</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Main Frame">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44879660-7429-8E51-7ACC-0266D9EECF3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="889000"/>
+          <a:ext cx="11303000" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="F1C40F"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="F1C40F"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Main Frame Header">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3DE4DF4-7B5A-1CD9-344A-118A81984E5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="889000"/>
+          <a:ext cx="11303000" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="D8336B"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="D8336B"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Workflows Requiring Attention</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Workflow No&quot;), &quot;UIForAction&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1535CC25-36D2-9FA8-50D5-F2BAED2B44DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1155700"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Workflow No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Name&quot;), &quot;UIForAction&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1660A44-DBF9-06DB-3D2E-6998F95651B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="1155700"/>
+          <a:ext cx="2540000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step No&quot;), &quot;UIForAction&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06D276C5-EE7D-8E8B-E36C-1C8A5F9801BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5969000" y="1155700"/>
+          <a:ext cx="2540000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Step No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step Name&quot;), &quot;UIForAction&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A5080D5-072B-E51C-6CEB-FADF821DD57D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8509000" y="1155700"/>
+          <a:ext cx="3683000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Step Name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Status&quot;), &quot;UIForAction&quot;'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FF71F05-E9CD-7A69-67EB-F93AC0B7B66D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1155700"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Status</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5169B0CB-DC3E-E2BB-D250-9603DF101D7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1422400"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19F6EE53-DE79-7BE9-8076-8C29A930C551}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="1422400"/>
+          <a:ext cx="2540000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Debs</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAB98A94-ADA1-067F-F16B-5B414DD1DEBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5969000" y="1422400"/>
+          <a:ext cx="2540000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.33</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00F28ABD-E476-480C-970E-2AED9EF90429}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8509000" y="1422400"/>
+          <a:ext cx="3683000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Completion</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="TextBox 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642660E8-5EC0-D413-B2C6-5E5F39F2A168}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1422400"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="D7263D"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="D7263D"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Action Req'd</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIScreenCom.ProcessBtnPress(6)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="BtnMain1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{462961E0-450B-8898-28C7-0D6E8A200102}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="190500"/>
+          <a:ext cx="1270000" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>New Workflow</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -479,7 +2384,7 @@
   <dimension ref="B2:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +2399,9 @@
     </row>
     <row r="15" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update steps and fix alt step
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4976773D-E625-46C0-AA08-4785AF5B6B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{453CB69D-7068-4F24-A581-9FB050DEF30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1020" windowWidth="21600" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -677,7 +677,7 @@
         <xdr:cNvPr id="2" name="Main Screen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E87AB3C-4E70-4F1A-D728-E7A6EC25F2DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B597D539-61F3-FD9C-FD96-9BD84EA715C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -819,7 +819,7 @@
         <xdr:cNvPr id="5" name="Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B58C004-D97B-1E60-9FEF-91F1EA398BEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF035D4-498B-4967-A40A-CB4F4CA961C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -879,7 +879,7 @@
         <xdr:cNvPr id="4" name="MenuBar">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE351E2-97D5-24F8-3236-0A778BCD1CEE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A0A6F2B-2B2E-0C4B-B0EB-8E265CF70098}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -968,7 +968,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C8A3B5-0EF3-95DC-7D1B-1A530F7F202A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B9F2C47-3E21-252A-CAB5-C9ECD5DA144B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1028,7 +1028,7 @@
         <xdr:cNvPr id="6" name="Logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AED57304-EA96-2F83-0E82-0E53A8814206}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF49AFA2-CAFA-C814-4030-425E84BD90FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1078,7 +1078,7 @@
         <xdr:cNvPr id="7" name="MenuItem - For Action">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE063F23-B147-4AF0-F056-C623F01AB650}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51F45FA9-C97B-AA31-EA6F-2FED087E6017}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1087,91 +1087,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1905000"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:srgbClr val="134F69"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>For Action</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(2)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="MenuItem - Active">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D7904E-598D-905F-EC93-0E3F24F6A8FE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2286000"/>
           <a:ext cx="1905000" cy="393700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1233,6 +1148,91 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
+            <a:t>For Action</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ProcessBtnPress(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="MenuItem - Active">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10AE81AC-7E10-3E45-E0E7-1FBCBE05AA6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2286000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="134F69"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t>Active</a:t>
           </a:r>
         </a:p>
@@ -1258,7 +1258,7 @@
         <xdr:cNvPr id="9" name="MenuItem - Complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DFAED3E-0FD1-4107-EB46-98F225AD0EA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9FD882A-08D3-81F0-0929-9BDE7A1E98E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,7 +1343,7 @@
         <xdr:cNvPr id="10" name="MenuItem - Exit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0549655B-8AC4-FE24-66E8-3DF06268CEA7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19158AC9-7ED1-8090-8195-E79D704476F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,15 +1420,15 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="12" name="Main Frame">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03B1BB3C-E52F-ABA0-60B0-679A8D4A457B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5B3E0D-7711-EF0C-ADA1-238F4ABA1DB1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1437,7 +1437,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2159000" y="889000"/>
-          <a:ext cx="11303000" cy="4572000"/>
+          <a:ext cx="11303000" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1526,7 +1526,7 @@
         <xdr:cNvPr id="11" name="Main Frame Header">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9D17A26-C0CE-546A-E17F-B28A0650E3C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F84B5AC-6820-F93E-BCEE-E246A8CB1709}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1596,7 +1596,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Active Workflows</a:t>
+            <a:t>Workflows Requiring Attention</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1616,12 +1616,12 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Workflow No&quot;), &quot;UIActive&quot;'" textlink="">
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Workflow No&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="14" name="TextBox 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5285ABA3-80DA-54C4-8A8F-D58854EE1809}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95EBB572-ADC3-2661-4690-1D364EB36B2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1707,12 +1707,12 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Name&quot;), &quot;UIActive&quot;'" textlink="">
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Name&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="15" name="TextBox 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B5C752-15D8-CB0B-0CE3-059B4E71E7CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3F79C4F-F926-9983-8081-19ED6F1EB1F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1798,12 +1798,12 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step No&quot;), &quot;UIActive&quot;'" textlink="">
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step No&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="TextBox 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D0AD52F-CA0D-572D-5A08-A0AC7F86FC40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8ED1510-02CB-AA81-13D2-629A5DE6FE4A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1889,12 +1889,12 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step Name&quot;), &quot;UIActive&quot;'" textlink="">
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step Name&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="17" name="TextBox 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47484D5F-35F0-2E1A-A6B2-EF8C33F53C72}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95CE746D-BD92-A3CF-1A5C-44E7D548AE54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1980,12 +1980,12 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Status&quot;), &quot;UIActive&quot;'" textlink="">
+    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Status&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="18" name="TextBox 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E46E0273-4226-4635-F44A-BDBFBD63B62F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7AA86A3-2B5E-B3A1-B1E1-3D30DE51972B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2060,6 +2060,458 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4159F71-5FEB-12E8-FD06-9C2F3E19EB2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1422400"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D35837FB-CE16-6FD3-0275-CD4DE6AEE9DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="1422400"/>
+          <a:ext cx="2540000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="434343"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A917674-AF20-3F33-A47F-0F39D2155303}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5969000" y="1422400"/>
+          <a:ext cx="2540000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.01</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FE32804-DED1-BCAE-F04D-0AEE25DAF48A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8509000" y="1422400"/>
+          <a:ext cx="3683000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Fact Find to Client</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="TextBox 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3088090-E8D2-24C2-85B7-6B8741ACE199}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1422400"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BAFF29"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="BAFF29"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Action Req'd</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -2076,7 +2528,7 @@
         <xdr:cNvPr id="13" name="BtnMain1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A41B61CD-7EF1-99CD-63D8-AB6E30AE7435}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2743F87D-24D0-809C-FD73-F66836359E17}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2742,7 +3194,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Probably messed up Workflow and step classes
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EF29587-46B4-464B-8789-99432EEC2E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8513F8C3-E36A-420C-A470-BD7D19851976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="4245" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18630" yWindow="1170" windowWidth="17430" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -659,6 +659,56 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4829" name="TEMPLATE - Logo" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD60F29-BC8A-CD9F-F23B-AD9C56698867}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24117300" y="2276475"/>
+          <a:ext cx="2235200" cy="1460500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -674,10 +724,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Main Screen">
+        <xdr:cNvPr id="19" name="Main Screen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C638FEF7-CC36-6FF6-E761-E369607BF1E2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB06C404-189A-DAC0-D966-902CE5B986E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -751,56 +801,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4829" name="TEMPLATE - Logo" hidden="1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD60F29-BC8A-CD9F-F23B-AD9C56698867}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="24117300" y="2276475"/>
-          <a:ext cx="2235200" cy="1460500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -816,10 +816,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4">
+        <xdr:cNvPr id="20" name="Rectangle 19" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89FDE453-FBFA-18AE-98EB-82494B0637F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E6AA0F9-21E3-28E8-85FA-7872A72537C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -876,10 +876,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="MenuBar">
+        <xdr:cNvPr id="21" name="MenuBar">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0F13501-549A-1797-DCD9-A18BC97D3506}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFA89F96-66AD-D851-C2C5-65A4F00AD7D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -965,10 +965,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1">
+        <xdr:cNvPr id="22" name="Rectangle 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C3B8645-BADC-DE78-E5A9-5B5AD4BC0EE5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A500877-C4D2-42D0-86F3-5590F3FC3ACD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1025,10 +1025,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Logo">
+        <xdr:cNvPr id="23" name="Logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85D04433-4D85-A893-5F1D-042C69007BA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E68B4684-C585-63BA-EE95-84334E1BB043}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1075,10 +1075,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="MenuItem - For Action">
+        <xdr:cNvPr id="24" name="MenuItem - For Action">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E32E2B-7AAC-35CE-82AF-059CD72C941C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{501B011A-4444-FEED-5EAA-48AAB2B110B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1095,30 +1095,20 @@
         <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
-              <a:srgbClr val="D8336B"/>
+              <a:srgbClr val="FFFFFF"/>
             </a:gs>
             <a:gs pos="100000">
-              <a:srgbClr val="D8336B"/>
+              <a:srgbClr val="FFFFFF"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
           <a:tileRect/>
         </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="134F69"/>
+          </a:solidFill>
         </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="134F69"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -1144,7 +1134,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1200" b="0">
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
@@ -1170,10 +1160,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="MenuItem - Active">
+        <xdr:cNvPr id="25" name="MenuItem - Active">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{532665A7-1F02-023B-B658-9D5E60FBC8EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF532E8B-8DD4-3932-3D5C-CF2181C30356}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,10 +1245,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="MenuItem - Complete">
+        <xdr:cNvPr id="26" name="MenuItem - Complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{268E8C95-B36C-B356-6DFA-89F4BD891E30}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55B2CFEF-5C54-7A41-779C-D6BBC85273F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1340,10 +1330,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="MenuItem - Exit">
+        <xdr:cNvPr id="27" name="MenuItem - Exit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54BED1F2-3333-B478-33CF-B16A322B999A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA2E2430-1D2F-1033-34CA-82AD15C1FD3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,15 +1410,15 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Main Frame">
+        <xdr:cNvPr id="28" name="Main Frame Header">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11BC2537-98CD-A992-FEEE-26DE7025EFFD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37EAF801-9F44-5869-1D2A-AFC27333D34F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1437,7 +1427,102 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2159000" y="889000"/>
-          <a:ext cx="11303000" cy="800100"/>
+          <a:ext cx="11303000" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="D8336B"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="D8336B"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Active Workflows</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Main Frame">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0753FA1B-68BC-3423-7B97-9EFB394995DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="889000"/>
+          <a:ext cx="11303000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1510,1008 +1595,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Main Frame Header">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF83E68-A1D5-289B-C2E2-845C0458C416}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2159000" y="889000"/>
-          <a:ext cx="11303000" cy="317500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="D8336B"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="D8336B"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Workflows Requiring Attention</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Workflow No&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE141846-3F86-151D-6919-10EFC4E4C4BB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2159000" y="1155700"/>
-          <a:ext cx="1270000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Workflow No</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Name&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="TextBox 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEDA832-13BF-035B-E69B-74F5746B8A39}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3429000" y="1155700"/>
-          <a:ext cx="2540000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Name</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step No&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="TextBox 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51038E00-D8DE-6E8B-7AA1-3697DE28C543}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5969000" y="1155700"/>
-          <a:ext cx="2540000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Step No</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step Name&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="TextBox 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6492139-561C-F4AE-FA72-3FA1F93747F9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8509000" y="1155700"/>
-          <a:ext cx="3683000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Step Name</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Status&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="TextBox 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61C2C69D-18C6-B980-BFB7-98CBD676C2B1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12192000" y="1155700"/>
-          <a:ext cx="1270000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Status</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="TextBox 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B83D3D7C-8DCC-6777-9B89-03341DD68422}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2159000" y="1422400"/>
-          <a:ext cx="1270000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="TextBox 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF150D0E-C67B-31C2-1278-BBA26273D7CC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3429000" y="1422400"/>
-          <a:ext cx="2540000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="434343"/>
-            </a:solidFill>
-            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="TextBox 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50A43516-4DAD-2F99-2D25-F1A02B9EDF08}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5969000" y="1422400"/>
-          <a:ext cx="2540000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>1.01</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="TextBox 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{312AA4F5-CE3A-D2B1-BEF0-757D63DA60C3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8509000" y="1422400"/>
-          <a:ext cx="3683000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Fact Find to Client</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="TextBox 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9551B35-2CC1-22D8-C035-CBB8CFCF52CA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12192000" y="1422400"/>
-          <a:ext cx="1270000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="D7263D"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="D7263D"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Action Req'd</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -2525,10 +1608,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIScreenCom.ProcessBtnPress(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="BtnMain1">
+        <xdr:cNvPr id="30" name="BtnMain1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53254784-FD35-5F53-D984-5F9D5CD5E5B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EB9C102-43DD-9B79-BD35-6C0E90EBE7AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3183,7 +2266,7 @@
   <sheetPr codeName="ShtMain"/>
   <dimension ref="B2:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
@@ -3194,7 +2277,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ClsUIMenu redesign and new ClsUITable
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58BC82AE-EE9A-44C3-B561-DBA8F430DFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EFBD953-480C-4B74-B917-B232FB966522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="17430" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43650" yWindow="3570" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TblStepTemplate!$C$1:$N$42</definedName>
+    <definedName name="Button">Sheet1!$B$2</definedName>
     <definedName name="MenuItem">Sheet1!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -674,10 +675,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="Main Screen">
+        <xdr:cNvPr id="2" name="Main Screen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FABE3DC1-8135-B74C-6A6E-805DBE4B3878}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE6319A9-0556-32C4-8271-DCDAE5EE277F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -816,10 +817,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="Rectangle 43">
+        <xdr:cNvPr id="5" name="Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F174C29D-77A9-9F6E-C2C9-835149F09E36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC4CE39E-1E83-4B84-6C6E-048B63A53DB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -876,10 +877,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="MenuBar">
+        <xdr:cNvPr id="4" name="MenuBar">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FDE716D-FE1F-CD2D-B3F7-CDC4FB97776D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52626E13-A87D-1279-5D5E-F0919C284133}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -965,10 +966,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="Rectangle 41" hidden="1">
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E85A2024-83FA-921C-E386-CFA77676EAD9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967A8540-27CC-6E9B-0C33-131ACBC8BEB1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1025,10 +1026,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="45" name="Logo">
+        <xdr:cNvPr id="6" name="Logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E2E9BA3-5D56-8750-8487-CACAB569B063}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6F427F6-35FB-D346-8A00-AD7E40C94CB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1075,10 +1076,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="MenuItem - For Action">
+        <xdr:cNvPr id="7" name="Button - For Action">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35EF731F-F431-8AEC-18EA-7DF63A9A7631}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE0F4A49-5674-3ADD-BBF2-A256BA915469}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1170,10 +1171,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="MenuItem - Active">
+        <xdr:cNvPr id="8" name="Button - Active">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1053AE2-AD38-2A3B-7C24-DB8577096ADB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC3339C-2C54-952A-7C45-9EE0EC7A8B32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,10 +1256,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="MenuItem - Complete">
+        <xdr:cNvPr id="9" name="Button - Complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D205D264-C56B-4D53-7AEC-1A557A739E93}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5922238-0176-F845-4E61-92390F7F2E2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1340,10 +1341,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ProcessBtnPress(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="MenuItem - Exit">
+        <xdr:cNvPr id="10" name="Button - Exit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8B03BB1-A960-4883-A9FA-421299BCAB12}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E29C4B85-F8F1-AFB9-89BB-C871BF0C37A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,15 +1421,15 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Main Frame">
+        <xdr:cNvPr id="12" name="Main Frame">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A91040FE-D32A-154F-D387-ABA9CF9AB1CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A52432BF-0985-2FBA-60BC-3B350C417272}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1437,7 +1438,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2159000" y="889000"/>
-          <a:ext cx="11303000" cy="800100"/>
+          <a:ext cx="11303000" cy="1066800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1523,10 +1524,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Main Frame Header">
+        <xdr:cNvPr id="11" name="Main Frame Header">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67D929F1-7341-EFA1-E438-9BB699AFBA08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BDB06D8-10BC-5865-F0AA-52ABDD1390E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1618,10 +1619,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Workflow No&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="53" name="TextBox 52">
+        <xdr:cNvPr id="14" name="TextBox 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5EE53D2-0DE6-38A4-C343-78B028D26C85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5404B414-9A1E-8297-4D6E-220FA5B36E04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1709,10 +1710,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Name&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="54" name="TextBox 53">
+        <xdr:cNvPr id="15" name="TextBox 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ACF7E6A-AE48-CBD1-4259-2617887A8AF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE623428-0428-F254-79CD-FB0B5CAE81C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1800,10 +1801,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step No&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="TextBox 54">
+        <xdr:cNvPr id="16" name="TextBox 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9EBA00C-9E46-2590-8E94-3655527ABF08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE8E177C-F2FA-9D13-0968-DB80762597BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1891,10 +1892,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step Name&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="56" name="TextBox 55">
+        <xdr:cNvPr id="17" name="TextBox 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60B0DE4F-0F60-8626-6069-8A29F36282AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D49F3D2F-3642-ED74-C263-F52125743D41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1982,10 +1983,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Status&quot;), &quot;UIForAction&quot;'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="57" name="TextBox 56">
+        <xdr:cNvPr id="18" name="TextBox 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E6BB31-72D5-CA6F-A5A2-949ACAD98FD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9789260-A2EB-C6F1-7DCE-288E80D65C1F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2073,10 +2074,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="58" name="TextBox 57">
+        <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0593DA95-4188-9D79-7500-0B27A303CFA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37B3ECE1-FDA9-B076-DB6B-1658D2B75937}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2164,10 +2165,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="59" name="TextBox 58">
+        <xdr:cNvPr id="20" name="TextBox 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BA22333-D9FE-D9CE-BC3F-0AD80A4ECD43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8EF9A1B-6ABE-19A6-9990-8BDE46707A37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2252,10 +2253,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="TextBox 59">
+        <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B55A84A-F880-1E84-9280-E09C7C98D908}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61DFA723-E62E-33F5-E85C-8806F2C3C1AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2343,10 +2344,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="61" name="TextBox 60">
+        <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B04DD94-871C-DE38-EB85-3FF59986257E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD79B3A8-8E0D-D8DF-9C23-B56941CA3ADC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2434,10 +2435,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="TextBox 61">
+        <xdr:cNvPr id="23" name="TextBox 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E229DFDF-FD53-1C93-A1CB-79F7C4BA2D78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2D5675C-3F91-D129-F031-ED7179CE7CBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2512,6 +2513,458 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04612271-D609-AA2C-0191-833852DC538F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1689100"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="TextBox 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D2E8F5C-1EC1-40C6-F48A-0097595B58A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="1689100"/>
+          <a:ext cx="2540000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0">
+            <a:solidFill>
+              <a:srgbClr val="434343"/>
+            </a:solidFill>
+            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="TextBox 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06A5CA11-0B9A-51CD-4EE8-EE3491892FE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5969000" y="1689100"/>
+          <a:ext cx="2540000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.01</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="TextBox 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3B46A75-BDCD-2300-5A54-398402126F57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8509000" y="1689100"/>
+          <a:ext cx="3683000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Fact Find to Client</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUiForAction.OpenWorkflow(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="TextBox 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{143892B3-8F1E-0F94-F585-E7153C3D0BF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1689100"/>
+          <a:ext cx="1270000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BAFF29"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="BAFF29"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Action Req'd</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -2525,10 +2978,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIScreenCom.ProcessBtnPress(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="BtnMain1">
+        <xdr:cNvPr id="13" name="BtnMain1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9A673F6-6054-C2D0-FE3F-9457C89C8A50}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6286727-8002-5C44-EB9B-F929A49366BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2605,913 +3058,6 @@
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>New Workflow</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Workflow No&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="63" name="TextBox 62">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DC8C025-1885-59DE-A7F8-1AAEC2C10197}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2159000" y="1155700"/>
-          <a:ext cx="1270000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Workflow No</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Name&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4800" name="TextBox 4799">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6140AC9-CAA4-A1F3-736D-DCB85C5CD8BF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3429000" y="1155700"/>
-          <a:ext cx="2540000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Name</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step No&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4801" name="TextBox 4800">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47737EAD-B2FA-4324-6946-6B727D1DC2D2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5969000" y="1155700"/>
-          <a:ext cx="2540000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Step No</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Step Name&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4802" name="TextBox 4801">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80EE48D4-D586-B7B0-86DE-A9177956B9ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8509000" y="1155700"/>
-          <a:ext cx="3683000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Step Name</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIScreenCom.SortBy(&quot;Status&quot;), &quot;UIForAction&quot;'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4803" name="TextBox 4802">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{010A3704-B447-CDE5-8716-618E10143F88}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12192000" y="1155700"/>
-          <a:ext cx="1270000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="134F69"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Status</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4804" name="TextBox 4803">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEB66681-16F8-CB85-9C7F-A0CA856F1284}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2159000" y="1422400"/>
-          <a:ext cx="1270000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4805" name="TextBox 4804">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25430E13-F106-7270-F374-54E71360FEFD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3429000" y="1422400"/>
-          <a:ext cx="2540000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="1000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="434343"/>
-            </a:solidFill>
-            <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4806" name="TextBox 4805">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA9F4EAE-B0C7-7C3C-59E0-30B58AE124E8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5969000" y="1422400"/>
-          <a:ext cx="2540000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>1.01</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4807" name="TextBox 4806">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F847AC36-8FEC-E1C1-3955-A4B0A19C8A36}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8509000" y="1422400"/>
-          <a:ext cx="3683000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Fact Find to Client</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUiForAction.OpenWorkflow(1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4808" name="TextBox 4807">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2B08C48-48A0-9A83-3324-E1296695930C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12192000" y="1422400"/>
-          <a:ext cx="1270000" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="BAFF29"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="BAFF29"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Action Req'd</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4090,8 +3636,8 @@
   <sheetPr codeName="ShtMain"/>
   <dimension ref="B2:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Starting to build in New UI Classes.  Need to get previous verion of xls to get table import
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E4E8D05-C452-4EBD-A5A6-EF8DAEE4FCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D38FA46-FAB2-495C-8832-00E376B7E422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="15345" xr2:uid="{00ACA1FB-AD02-4E9F-8F74-E5C81A868DC7}"/>
+    <workbookView xWindow="-27855" yWindow="2745" windowWidth="28800" windowHeight="15345" xr2:uid="{00ACA1FB-AD02-4E9F-8F74-E5C81A868DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
implementing first project workflow
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50f47e56877e2071/Documents/Development Areas/CBS Workflow/Library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BE4496D-B724-458C-AF2B-8F16F49D494B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90184CBE-039E-4A45-8372-2391E99FEA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TblStepTemplate!$C$1:$N$42</definedName>
     <definedName name="Button">Sheet1!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcMode="manual"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -723,10 +723,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Main Screen">
+        <xdr:cNvPr id="28" name="Main Screen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D2409D-79E9-C133-A21F-16B6A914590E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C067997C-927E-838B-7A75-39CA878D52AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -815,10 +815,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1">
+        <xdr:cNvPr id="29" name="Rectangle 28" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8A6F988-FCDB-6FB1-08CF-F9BAB112E22C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{009B909C-BB44-CA85-82CA-E5ECABFD6976}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -875,10 +875,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="MenuBar">
+        <xdr:cNvPr id="30" name="MenuBar">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52024DB0-723E-8CDC-765C-C6EAEAB25F7D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D93C9B-9ECD-E55C-62F1-F4E577257AEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -964,10 +964,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4">
+        <xdr:cNvPr id="31" name="Rectangle 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7191349-1FCF-DB20-4750-BB9D92167776}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B80A5F77-E96F-37C7-82A0-9C1B6AA5E94B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1024,10 +1024,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Logo">
+        <xdr:cNvPr id="32" name="Logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{943CD819-2AB4-058C-6C2F-1FCA1BB80F48}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C4A1C07-5616-4C15-6A49-C0436AF6CF75}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1074,10 +1074,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Menu Btn - 1">
+        <xdr:cNvPr id="33" name="Menu Btn - 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F22D6C4D-7E00-0145-2E10-BABB26F320D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FF36EDD-D1F0-9314-A2DA-927ACBF20C38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1169,10 +1169,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Menu Btn - 2">
+        <xdr:cNvPr id="34" name="Menu Btn - 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{975B8134-6FDC-D9B3-7E82-EF8E3D217E69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A83DB015-1E6A-AD5E-7A7E-C55EE6FEFB02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1254,10 +1254,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Menu Btn - 2.1" hidden="1">
+        <xdr:cNvPr id="35" name="Menu Btn - 2.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A8FDCDA-F131-0CF0-C963-BD65FEC7DE81}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75153D3F-DE6C-A345-7E73-A7817D5E97CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1339,10 +1339,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Menu Btn - 2.2" hidden="1">
+        <xdr:cNvPr id="36" name="Menu Btn - 2.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A04F021F-31A2-ED5F-FFA8-F2444408BBEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E21A7A2-F6A3-488B-F87E-4C74B59DE02B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,10 +1424,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Menu Btn - 3">
+        <xdr:cNvPr id="37" name="Menu Btn - 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A57FB4D8-CA01-F29D-9F7D-0E4BD7AC607B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B138716E-79F9-5622-52FE-B1A0B7EB26B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1509,10 +1509,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Menu Btn - 3.1" hidden="1">
+        <xdr:cNvPr id="38" name="Menu Btn - 3.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1966C32C-ACA7-C8F3-FB9D-1551DECFB984}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED0EBB96-EF25-8678-732A-E6AEF3A96E31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1594,10 +1594,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Menu Btn - 3.2" hidden="1">
+        <xdr:cNvPr id="39" name="Menu Btn - 3.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{682E420C-234B-94B6-78A5-B2B0B82C575A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B14C3423-F4C5-BCE1-B2B3-CA5B88CDE0BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1679,10 +1679,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Menu Btn - 3.3" hidden="1">
+        <xdr:cNvPr id="40" name="Menu Btn - 3.3" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88767E3D-F4EC-A065-F047-81355B00B567}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A02EBA1-F39B-D2F4-C290-4E08957A0CFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1764,10 +1764,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Menu Btn - 3.4" hidden="1">
+        <xdr:cNvPr id="41" name="Menu Btn - 3.4" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{549BB7C1-53FE-4BDE-2063-4AEE32A29499}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6468D6EB-572E-3486-00DB-19CE551A133D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1849,10 +1849,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Menu Btn - 3.5" hidden="1">
+        <xdr:cNvPr id="42" name="Menu Btn - 3.5" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0C6A246-69EB-AC90-EB64-00849F80F8B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7031FBFE-15C7-2E5C-F9A5-3778E2C39F4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1934,10 +1934,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Menu Btn - 4">
+        <xdr:cNvPr id="43" name="Menu Btn - 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68974946-A575-79AF-6695-BC89CC2CD776}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CD8BBF3-95A9-0A4D-ED6E-677B96FCA12B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2019,10 +2019,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Menu Btn - 5">
+        <xdr:cNvPr id="44" name="Menu Btn - 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCA258FF-4D44-4FAD-823F-BC5BD50688F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3F54961-8039-011F-8535-2C26F2E435AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2104,10 +2104,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Menu Btn - 6">
+        <xdr:cNvPr id="45" name="Menu Btn - 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E989FAF-2C3C-C42E-1CFD-CFDB03D0E692}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D9BAFA8-8831-24E3-6642-654B7D695945}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2189,10 +2189,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Menu Btn - 6.1" hidden="1">
+        <xdr:cNvPr id="46" name="Menu Btn - 6.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F38A5582-6D2B-B49A-20B4-0F14BAE6AF7A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7833FF49-0D2D-9D90-16A6-0CB1810B30BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2274,10 +2274,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Menu Btn - 6.2" hidden="1">
+        <xdr:cNvPr id="47" name="Menu Btn - 6.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{848FFB65-328B-8E2A-B9DE-B73A1A046572}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8240A8A7-C2C3-E305-3F0B-FC18F52CED07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2359,10 +2359,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Menu Btn - 6.3" hidden="1">
+        <xdr:cNvPr id="48" name="Menu Btn - 6.3" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A816C802-49DF-6192-10AC-6245ED42E458}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E45C7AF-C8CE-771B-32E3-29369D54BF63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2444,10 +2444,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Menu Btn - 6.4" hidden="1">
+        <xdr:cNvPr id="49" name="Menu Btn - 6.4" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71B6DA56-A933-E1FE-DFCA-EC8B25D377D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{552B179B-5E22-9893-F5F7-C5BC228A1C4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2529,10 +2529,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Menu Btn - 6.5" hidden="1">
+        <xdr:cNvPr id="50" name="Menu Btn - 6.5" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{496B1C70-43F3-F75A-4E3F-7D140EB87E13}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16CE0CA0-EB01-2026-559F-FD658530FCFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2614,10 +2614,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Menu Btn - 6.6" hidden="1">
+        <xdr:cNvPr id="51" name="Menu Btn - 6.6" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A48710A-2A89-5754-970D-86D69FA74687}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E1463EB-D746-5CE4-D905-8A3D797F7471}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2699,10 +2699,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Menu Btn - 6.7" hidden="1">
+        <xdr:cNvPr id="52" name="Menu Btn - 6.7" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{546D4AAF-7700-3627-52DB-5385D1F7F83B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16B5FEDA-566E-0E31-F366-90DA3E28D212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2784,10 +2784,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Menu Btn - 7">
+        <xdr:cNvPr id="53" name="Menu Btn - 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8B5AEA-744A-8D51-32CB-E2CB703B92DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9265344D-55AA-7CA0-8F15-F09CB281A73F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3427,7 +3427,7 @@
   <dimension ref="B2:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Admin page and start of CRM
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1D47054-282C-4E99-98CD-1C5C4006B71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4497D5A6-527B-43BF-B757-C9CD40A407D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1455" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
-    <sheet name="TblStepTemplate" sheetId="7" state="hidden" r:id="rId2"/>
+    <sheet name="To Do" sheetId="8" r:id="rId2"/>
+    <sheet name="TblStepTemplate" sheetId="7" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TblStepTemplate!$C$1:$N$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TblStepTemplate!$C$1:$N$42</definedName>
     <definedName name="Button">Sheet1!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="174">
   <si>
     <t>WorkflowNo</t>
   </si>
@@ -525,13 +526,46 @@
   </si>
   <si>
     <t>Workflow has now completed</t>
+  </si>
+  <si>
+    <t>Align button text</t>
+  </si>
+  <si>
+    <t>Align button frame</t>
+  </si>
+  <si>
+    <t>Selected button to stay highlighted</t>
+  </si>
+  <si>
+    <t>remove form titles</t>
+  </si>
+  <si>
+    <t>Revisit instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefill data picker list </t>
+  </si>
+  <si>
+    <t>Client name on project form</t>
+  </si>
+  <si>
+    <t>Spv name on project form</t>
+  </si>
+  <si>
+    <t>Remove duplicate projects from list</t>
+  </si>
+  <si>
+    <t>restructure Class Hierarchy</t>
+  </si>
+  <si>
+    <t>Add RAG Colours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +588,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Myriad"/>
     </font>
   </fonts>
   <fills count="3">
@@ -614,7 +653,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -631,6 +670,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,56 +698,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4829" name="TEMPLATE - Logo" hidden="1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD60F29-BC8A-CD9F-F23B-AD9C56698867}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="24117300" y="2276475"/>
-          <a:ext cx="2235200" cy="1460500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -723,10 +713,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Main Screen">
+        <xdr:cNvPr id="10052" name="Main Screen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E9CAEAA-046C-3868-5C07-322DE44D7779}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F364260F-54E3-23D4-5F0C-B7C9818CF959}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -800,6 +790,56 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4829" name="TEMPLATE - Logo" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD60F29-BC8A-CD9F-F23B-AD9C56698867}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24117300" y="2276475"/>
+          <a:ext cx="2235200" cy="1460500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -815,10 +855,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1">
+        <xdr:cNvPr id="10055" name="Rectangle 10054">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7535C162-0075-4BEE-892C-6A84D537405A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{572FA403-75B0-9707-E931-F46C1D340E52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -862,6 +902,2452 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10079" name="Main Frame">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D03F3274-51D3-84B0-C6D1-9656A0E2C364}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1143000"/>
+          <a:ext cx="8890000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10078" name="Main Frame Header">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E308708-699B-0873-C629-E0C674BC4B69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1143000"/>
+          <a:ext cx="8890000" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="D8336B"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="D8336B"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Active Projects</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10084" name="0-0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC443AA5-C11C-F705-13E6-382E5EF6A3CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1460500"/>
+          <a:ext cx="635000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Project No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10085" name="1-0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76C5D4FB-BFB9-8905-7B1D-5D54F4C34360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2794000" y="1460500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Client Name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10086" name="2-0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4BDC3F9-4089-3A80-CF4A-66B968DB1BFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4064000" y="1460500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SPV No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10087" name="3-0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBBF7FF-AEC7-E035-FE44-0AC7C77D4182}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334000" y="1460500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Case Manager</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10088" name="4-0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DF4F6F4-5535-11D6-4551-0FEF3EAA2730}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604000" y="1460500"/>
+          <a:ext cx="635000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Step No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10089" name="5-0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB6EF5F-492D-2BE8-5EDC-61CEC471D16B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7239000" y="1460500"/>
+          <a:ext cx="2540000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Step Name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10090" name="6-0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E5322B4-ED5E-D7A0-73B2-F70E2AA372E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9779000" y="1460500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="134F69"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Status</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10091" name="0-1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{569A590A-E8AA-A225-31CC-7A23216091FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1714500"/>
+          <a:ext cx="635000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10092" name="1-1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{864A0761-67C8-2CBD-F986-A982CAC40352}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2794000" y="1714500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Sainsburys</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10093" name="2-1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{111C4B9B-EFB0-1801-3753-E90E8CAF8C30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4064000" y="1714500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Old SPV</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10094" name="3-1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{661FF2CD-EB23-DFC1-C795-934EE547AEC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334000" y="1714500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Fred Bloggs</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10095" name="4-1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E2F76AF-4EC6-269E-79CC-06426092C4D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604000" y="1714500"/>
+          <a:ext cx="635000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.01</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10096" name="5-1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A48D2B7-A800-3DD1-DB2A-46A8D9FBC446}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7239000" y="1714500"/>
+          <a:ext cx="2540000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Fact Find to Client</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10097" name="6-1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B08E418-DF8C-22D9-3551-2B74C6E161B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9779000" y="1714500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="D7263D"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="D7263D"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>enActionReqd</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10098" name="0-2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F42F479-F22B-3FAF-FC07-7978F87E0212}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159000" y="1968500"/>
+          <a:ext cx="635000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10099" name="1-2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD65B0AA-1D76-3556-DE5E-78EFCA9DAA8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2794000" y="1968500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Sainsburys</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10100" name="2-2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3049B77B-F17E-78AC-75D7-4179601DF0C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4064000" y="1968500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Old SPV</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10101" name="3-2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06CE0976-C4C6-C6A7-D69E-E87F8C89F62D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334000" y="1968500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Fred Bloggs</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10102" name="4-2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE784549-FDA3-3EFC-189D-A9786A93146F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604000" y="1968500"/>
+          <a:ext cx="635000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1.17</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10103" name="5-2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0EF8058-D928-BA3A-9351-BDE01EC2DE96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7239000" y="1968500"/>
+          <a:ext cx="2540000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="434343"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Agree next steps with Client</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(&quot;10:1&quot;)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10104" name="6-2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F86416-3D68-51F6-98A8-8554FD71F7E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9779000" y="1968500"/>
+          <a:ext cx="1270000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="D7263D"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="D7263D"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>enActionReqd</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10081" name="Button Frame" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1890C26-DE04-70D5-C0B6-65FB03D13F22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10033000" y="63500"/>
+          <a:ext cx="3492500" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FFFFFF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface=""/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10080" name="Rectangle 10079" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C0E5322-4C4E-B455-75E8-F2641AD1D02B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="127000" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(7)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10082" name="BtnMain1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A7AF40-3E94-D172-32FF-2D7B660E501F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10414000" y="317500"/>
+          <a:ext cx="1270000" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="134F69"/>
+        </a:solidFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>New Project Workflow</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIButtons.ProcessBtnClicks(8)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10083" name="BtnMain2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EC53D2B-10B8-E2AE-37DC-8C57EA4FBC11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12001500" y="317500"/>
+          <a:ext cx="1270000" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="134F69"/>
+        </a:solidFill>
+        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>New Lender Workflow</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -875,10 +3361,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="MenuBar">
+        <xdr:cNvPr id="10054" name="MenuBar">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7539466-7721-FFA3-96F7-A4B69DD833CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9D1C000-34B6-DD8A-EC01-6C27162C8A50}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -964,10 +3450,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4">
+        <xdr:cNvPr id="10053" name="Rectangle 10052" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A07DD489-6FCF-B040-0AAE-647B52444180}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBD3F095-E117-47C0-26F9-6354CB4F3E40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1024,10 +3510,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Logo">
+        <xdr:cNvPr id="10056" name="Logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AEC7E13-9C65-A9A2-D6C0-B672BA04EFFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0E3F2C6-9987-2420-2EB1-7302442798D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1074,10 +3560,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Menu Btn - 1">
+        <xdr:cNvPr id="10057" name="Menu Btn - 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8243A78-9232-957F-0D3A-7372C66F3F7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{647C3D4B-2CFC-52B2-0F99-FDDC1332EFE4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1086,6 +3572,162 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="63500" y="1905000"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="134F69"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>For Action</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10058" name="Menu Btn - 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99137D08-314A-D603-F330-25FC8DAD53C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="63500" y="2298700"/>
+          <a:ext cx="1905000" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="134F69"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Projects</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.1)'" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10059" name="Menu Btn - 2.1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45006965-2E76-D9F2-2EE3-6CCF6872F0A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1968500" y="2298700"/>
           <a:ext cx="1905000" cy="393700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1138,158 +3780,6 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>For Action</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Menu Btn - 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B877187D-4590-B8FD-8FC3-C0C3C06818DF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="63500" y="2298700"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:srgbClr val="134F69"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Projects</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.1)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Menu Btn - 2.1" hidden="1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF52C01F-D1D4-DD70-AE76-8F50078F99F5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1968500" y="2298700"/>
-          <a:ext cx="1905000" cy="393700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:srgbClr val="134F69"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200" b="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
             <a:t>Active</a:t>
           </a:r>
         </a:p>
@@ -1312,10 +3802,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Menu Btn - 2.2" hidden="1">
+        <xdr:cNvPr id="10060" name="Menu Btn - 2.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D43462B3-2153-6C7A-FA80-56A30732C13D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AC86CC8-D410-42E6-F0A7-C6FE82A5FA47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1388,10 +3878,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Menu Btn - 3">
+        <xdr:cNvPr id="10061" name="Menu Btn - 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AD1FDE6-0990-831D-1E1A-781C564A6A44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50772403-1CDD-DC71-5E3A-0668856888C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1464,10 +3954,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Menu Btn - 3.1" hidden="1">
+        <xdr:cNvPr id="10062" name="Menu Btn - 3.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87004E3F-9AC5-C5E6-5C3E-F5816C7A66AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D84F4C9-A171-4530-76D1-4357BEB3B122}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1540,10 +4030,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Menu Btn - 3.2" hidden="1">
+        <xdr:cNvPr id="10063" name="Menu Btn - 3.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7DE4179-9843-6B27-F412-F886FE753B16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89B246D4-1577-BE67-8367-429A7493FDDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1616,10 +4106,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Menu Btn - 3.3" hidden="1">
+        <xdr:cNvPr id="10064" name="Menu Btn - 3.3" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53E575B1-F82A-713E-D4AD-8684F6114C02}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F33B139-1756-4D22-36A1-CDB663336CA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1692,10 +4182,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Menu Btn - 3.4" hidden="1">
+        <xdr:cNvPr id="10065" name="Menu Btn - 3.4" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFB8F904-E4B3-B3B0-5FA3-6E226B8C9E5F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4A6C06B-1CD0-F3D4-4BE0-81660AE40CDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1768,10 +4258,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Menu Btn - 3.5" hidden="1">
+        <xdr:cNvPr id="10066" name="Menu Btn - 3.5" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74AB5207-AD2B-9F4B-9185-5311F57F6C17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F32DEAB-F3F4-1038-0FF2-79C13AB95075}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1844,10 +4334,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Menu Btn - 4">
+        <xdr:cNvPr id="10067" name="Menu Btn - 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A683DD3-AA94-4FA2-F608-D8CE4F0D0640}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF4CBC7D-76B6-6622-29BB-028F2403254F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1920,10 +4410,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Menu Btn - 5">
+        <xdr:cNvPr id="10068" name="Menu Btn - 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2FEB144-88A0-78DC-18E3-1B8379336DEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA39EBE7-4D80-549D-C535-FCA314854654}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1996,10 +4486,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Menu Btn - 6">
+        <xdr:cNvPr id="10069" name="Menu Btn - 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AF33C5E-38F4-FB9E-6235-8A0B1EB57A61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA081E3B-0494-3A76-069B-0D01BDF5254E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2072,10 +4562,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Menu Btn - 6.1" hidden="1">
+        <xdr:cNvPr id="10070" name="Menu Btn - 6.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F62AE3-FC19-338A-0786-670C2DCA8E4A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{190BACA0-532F-6D6E-E8DE-724E68384BC3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2148,10 +4638,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Menu Btn - 6.2" hidden="1">
+        <xdr:cNvPr id="10071" name="Menu Btn - 6.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78748C6E-C4FD-871D-DB86-AB1A8C89A11A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CCFAF65-7BAA-58BC-0F10-FED599C3B89A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2224,10 +4714,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Menu Btn - 6.3" hidden="1">
+        <xdr:cNvPr id="10072" name="Menu Btn - 6.3" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B01FC50-F8BA-C5C8-7411-5E6FAA5D1C8F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{051ACB86-248C-F0E0-A2F7-8ACAA656905C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2300,10 +4790,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Menu Btn - 6.4" hidden="1">
+        <xdr:cNvPr id="10073" name="Menu Btn - 6.4" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C07173A-05C3-07DB-C007-ADEA6E3C7277}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCB4C3AF-3EA0-468B-EDBB-9573A9CDE65C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2376,10 +4866,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Menu Btn - 6.5" hidden="1">
+        <xdr:cNvPr id="10074" name="Menu Btn - 6.5" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB985045-2958-6616-6810-3978F2D5F301}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3FA258-49B9-470E-D382-0A70DB6F1D7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2452,10 +4942,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Menu Btn - 6.6" hidden="1">
+        <xdr:cNvPr id="10075" name="Menu Btn - 6.6" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A1A0ABF-FE96-43DD-C58F-CCB1E39D9427}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D0CEC81-7CCB-23AA-E027-6A3568A7489F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2528,10 +5018,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Menu Btn - 6.7" hidden="1">
+        <xdr:cNvPr id="10076" name="Menu Btn - 6.7" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118D6F2D-A438-E766-1ACC-9C198EFB4C31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC830120-7E15-B6CD-84A8-6EDD7D2F5D6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2604,10 +5094,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Menu Btn - 7">
+        <xdr:cNvPr id="10077" name="Menu Btn - 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36DDB9F1-A0B4-7D11-6B8E-F64EDFD6B71C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58C53F4F-7937-519A-0A68-64BC9482B918}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3238,21 +5728,25 @@
   <dimension ref="B2:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:2">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="15" spans="2:2" ht="14.25" customHeight="1"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="LIxcXN9cfsxSeBRXsakILRqyLNnQ4yqDq9nbajkEdD2X2LtDKan9zPRC3il9WupbRHh65Y+mKtbRSdZnU2i/8Q==" saltValue="kIq0vMxHoqjzIgrScPeiCg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3261,6 +5755,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF5DD8E-1975-411A-A399-0A0AA8DBB752}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:C11">
+    <sortCondition ref="C1:C11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBF781-377D-4D51-BB7A-ACB62E9EAE6C}">
   <sheetPr codeName="ShtTableImport"/>
   <dimension ref="A1:Y42"/>
@@ -3269,7 +5874,7 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="36.7109375" customWidth="1"/>
@@ -3281,7 +5886,7 @@
     <col min="19" max="25" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3358,7 +5963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3408,7 +6013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3455,7 +6060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3502,7 +6107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3545,7 +6150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3586,7 +6191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3633,7 +6238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3674,7 +6279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3721,7 +6326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3768,7 +6373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3815,7 +6420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="30">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3862,7 +6467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3909,7 +6514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3956,7 +6561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -4003,7 +6608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -4050,7 +6655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -4093,7 +6698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -4140,7 +6745,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -4187,7 +6792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -4234,7 +6839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="30">
       <c r="A21">
         <v>1</v>
       </c>
@@ -4284,7 +6889,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -4331,7 +6936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -4378,7 +6983,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -4425,7 +7030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -4472,7 +7077,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -4519,7 +7124,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -4566,7 +7171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -4613,7 +7218,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -4660,7 +7265,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -4701,7 +7306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -4748,7 +7353,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -4795,7 +7400,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -4842,7 +7447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -4883,7 +7488,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="45">
       <c r="A35">
         <v>1</v>
       </c>
@@ -4933,7 +7538,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -4974,7 +7579,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -5021,7 +7626,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="45">
       <c r="A38">
         <v>1</v>
       </c>
@@ -5071,7 +7676,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -5118,7 +7723,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="30">
       <c r="A40">
         <v>1</v>
       </c>
@@ -5166,7 +7771,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="45">
       <c r="A41">
         <v>1</v>
       </c>
@@ -5214,7 +7819,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25">
       <c r="A42">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Started user level security
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8709157-24AC-42F9-86FC-5EB24BCDA55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{272175BD-3E5C-478A-B45C-936A9D5AD5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45105" yWindow="1725" windowWidth="18570" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="1800" windowWidth="20130" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -709,10 +709,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6236" name="Main Screen">
+        <xdr:cNvPr id="2" name="Main Screen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED164C75-7A8B-0D2E-B70F-2644478B6F50}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5566212-AD1B-8259-BF52-E45A98C7FCBC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -851,10 +851,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6241" name="Rectangle 6240">
+        <xdr:cNvPr id="7" name="Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4973E8D2-EB94-CCC7-E8E5-E004B542861F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28CBCB09-3C5A-A465-9414-427195C3841C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -911,54 +911,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6270" name="ExpandIcon">
+        <xdr:cNvPr id="36" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1236DC9-4A7A-1896-9358-D99FA1D3FD10}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:link="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1588" cy="1588"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1588</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1588</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6430" name="ExpandIcon">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53DC7430-6A90-354E-09BA-0DE76EDB6B3E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB1C3C67-6C35-7174-AB12-E92F18AA9F97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -999,10 +955,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6424" name="Main Frame">
+        <xdr:cNvPr id="30" name="Main Frame">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2742787-7E95-C9F1-2831-A489D9DE0D77}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC784F45-EF59-71D4-4281-C69CDA831104}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1097,10 +1053,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6423" name="Main Frame Header">
+        <xdr:cNvPr id="29" name="Main Frame Header">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C789BB51-A08E-E806-136D-DE4FFB06820C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFF0DEA6-790E-9EC9-857E-FA1803DABDF7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1192,10 +1148,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6431" name="0-0">
+        <xdr:cNvPr id="37" name="0-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F64D0044-AB3D-CE41-1C25-4EE92EAD98D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46EB016E-E0E2-6064-ED2E-6F5B0E9E567F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1283,10 +1239,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6432" name="1-0">
+        <xdr:cNvPr id="38" name="1-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23318E37-01E2-3CF1-EE70-03A531123838}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A792F9D-F89A-F9F4-543B-E4688038229F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1374,10 +1330,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6433" name="2-0">
+        <xdr:cNvPr id="39" name="2-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{273FE503-FD2C-ED4E-5780-109026C0058E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7702F227-AEE2-5BEF-2BDD-A2132A0D43BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1465,10 +1421,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6434" name="3-0">
+        <xdr:cNvPr id="40" name="3-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCE4AB3E-5106-C261-E4E5-D819747917B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF090BB-7A77-5885-04C4-F9938006212B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1556,10 +1512,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6435" name="4-0">
+        <xdr:cNvPr id="41" name="4-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9009AA4-22A5-A00F-8553-607379311DE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50D59350-CD5A-2CA3-9919-9DE093D0EED7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1647,10 +1603,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6436" name="5-0">
+        <xdr:cNvPr id="42" name="5-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFED9547-4BB8-4380-98E6-F29FE3D9E39E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69E2A2FD-C452-A342-A07C-BD83CB0842CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1738,10 +1694,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6437" name="6-0">
+        <xdr:cNvPr id="43" name="6-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8B5F62E-FAF5-A72D-E22E-C425CA330287}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA35450-8D22-DC16-3C61-AE21BDA8AE7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1829,10 +1785,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6438" name="7-0">
+        <xdr:cNvPr id="44" name="7-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA846D47-A23A-60D3-27F4-87D67B3EC4C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2567BC5-0B48-96BC-C0EB-FD66FEB8F7FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1920,10 +1876,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6439" name="0-1">
+        <xdr:cNvPr id="45" name="0-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1543D2A-0C2C-8194-E5FA-00470182A12C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{852F1382-0235-4E64-D927-E750FAE2B384}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2008,10 +1964,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;1:1&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6440" name="ExpandIcon">
+        <xdr:cNvPr id="46" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36440123-6F7D-FAB8-8390-DBF794B6F8EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E909E5-27B9-0DBA-6780-CBCF9D866AD3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2052,10 +2008,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6441" name="1-1">
+        <xdr:cNvPr id="47" name="1-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3240992F-8161-446E-53E6-994D3B351805}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8FB7056-52B0-E66D-2C53-8E5D8F27F640}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2143,10 +2099,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6442" name="2-1">
+        <xdr:cNvPr id="48" name="2-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2170CF0D-DF19-922C-08A3-814C5037B4BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA218B51-A465-5B8B-15E0-ADC519853C9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2234,10 +2190,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6443" name="3-1">
+        <xdr:cNvPr id="49" name="3-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26228F9C-E26B-8C3C-78F5-4793C3DF3EB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B69A298-7856-BAA3-D417-249057B70380}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2325,10 +2281,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6444" name="4-1">
+        <xdr:cNvPr id="50" name="4-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3AD4F2C-FA6D-4936-9FEF-5B18A3A3E02F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19478158-AB36-D20A-8B9E-26C8D5293F10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2416,10 +2372,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6445" name="5-1">
+        <xdr:cNvPr id="51" name="5-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0C44303-600C-5486-78CD-C88EC0C506D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B9FDA9-D812-935C-4E29-E038BB664AEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2507,10 +2463,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6446" name="6-1">
+        <xdr:cNvPr id="52" name="6-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FFF54A8-7C4C-C5D0-DEEB-29619AF07A88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CAA004A-7203-E16B-5943-4F99E5BF6FC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2598,10 +2554,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6447" name="7-1">
+        <xdr:cNvPr id="53" name="7-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6673404-0E61-8989-9DB0-35F591F34C1A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{112932F2-9878-BCD3-79B2-138A38994B62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2618,10 +2574,10 @@
         <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
-              <a:srgbClr val="BAFF29"/>
+              <a:srgbClr val="D7263D"/>
             </a:gs>
             <a:gs pos="100000">
-              <a:srgbClr val="BAFF29"/>
+              <a:srgbClr val="D7263D"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
@@ -2663,7 +2619,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0">
               <a:solidFill>
-                <a:srgbClr val="434343"/>
+                <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
@@ -2689,10 +2645,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;2:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6448" name="0-2">
+        <xdr:cNvPr id="54" name="0-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8BC6950-E0E8-6A90-6AB8-AE0108C7EF7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B4942A0-689B-2586-5202-20A11254CCAB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2777,10 +2733,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;2:2&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6449" name="ExpandIcon">
+        <xdr:cNvPr id="55" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB23A9CC-87A4-2E45-7BFE-E269434A0D1F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55DA20AA-C25F-7D72-1AB6-074A4C396AE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2821,10 +2777,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6450" name="1-2">
+        <xdr:cNvPr id="56" name="1-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C59A7F10-9892-C02C-1BDF-D2690CE104C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5049944B-7DA8-7A84-D86C-542D2C2BFBA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2912,10 +2868,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6451" name="2-2">
+        <xdr:cNvPr id="57" name="2-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDB02053-872F-4466-8471-489C29B2A537}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA07D4D4-C739-CE42-27CF-E7B350D6D907}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3003,10 +2959,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6452" name="3-2">
+        <xdr:cNvPr id="58" name="3-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFCF9330-F0B4-3E79-204B-553A7AC6DF17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{350269EA-94AA-E963-E76A-D7A15D47FE05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3094,10 +3050,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6453" name="4-2">
+        <xdr:cNvPr id="59" name="4-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE1B2BA-0D8C-BB34-B3F6-8CB87823D4A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46959334-86CB-0071-233F-2B2FCD641D75}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3185,10 +3141,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6454" name="5-2">
+        <xdr:cNvPr id="60" name="5-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A11B2F-0815-026A-E704-601708FCCC2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21A69191-D607-BB30-7BAA-5368B99DC1F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3276,10 +3232,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6455" name="6-2">
+        <xdr:cNvPr id="61" name="6-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83EBD35F-2285-C910-18DB-79BD2B20EAC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{348A35BF-2ABC-7D44-D280-588C1FA1E550}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3367,10 +3323,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6456" name="7-2">
+        <xdr:cNvPr id="62" name="7-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{862F37CD-F26C-1DFE-8B86-536B9A8BC208}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114B136B-EDC1-CF00-B8C0-110AF3ECDA48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3458,10 +3414,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;3:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6457" name="0-3">
+        <xdr:cNvPr id="63" name="0-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA251CA3-A9EF-068B-2452-BFEC163901DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{255A6850-0F46-4644-EDD5-5E74FF59D92C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3546,10 +3502,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;3:3&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6458" name="ExpandIcon">
+        <xdr:cNvPr id="4800" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C123A9B3-3122-D065-3237-88839F23D89C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FFD0835-E32C-F0DE-6337-4CCD7CD286E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3590,10 +3546,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6459" name="1-3">
+        <xdr:cNvPr id="4801" name="1-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3613606D-4EFB-6156-C399-176418FC5627}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E919E93-0894-5134-A9E8-828B87785E7A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3681,10 +3637,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6460" name="2-3">
+        <xdr:cNvPr id="4802" name="2-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD8B4918-A498-855A-360B-829465338265}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEF2E1F-7DC3-65AB-9870-D537CC0226E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3772,10 +3728,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6461" name="3-3">
+        <xdr:cNvPr id="4803" name="3-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69FB2A62-2BCF-EC6E-5CE4-C271699C8AA2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{328E97D6-BD22-13EC-A841-A80E359DA115}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3863,10 +3819,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6462" name="4-3">
+        <xdr:cNvPr id="4804" name="4-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96CAB2CD-BD25-1E57-A6C9-CBA8C5347C4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50420D30-42E3-CECF-F260-342E4BB2510A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3954,10 +3910,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6463" name="5-3">
+        <xdr:cNvPr id="4805" name="5-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85EF2F33-2DA4-54AA-32D8-E6FEDE28BEA4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6165FA09-8C01-93DB-1B6F-93C7093B509D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4023,7 +3979,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>1.01</a:t>
+            <a:t>1.20</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4045,10 +4001,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6464" name="6-3">
+        <xdr:cNvPr id="4806" name="6-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF7FCAD-B568-1F52-4048-9F58812AD42C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA5FB331-78F6-E53D-BFDC-67AED5AC2DEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4114,7 +4070,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fact Find to Client</a:t>
+            <a:t>Workflow has completed</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4136,10 +4092,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6465" name="7-3">
+        <xdr:cNvPr id="4807" name="7-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADEBF57-DC81-F6BF-3BEF-58430448B5A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5DD403E-CA5A-FC6F-23C8-1C349B3588E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4156,10 +4112,10 @@
         <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="F1C40F"/>
             </a:gs>
             <a:gs pos="100000">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="F1C40F"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
@@ -4201,11 +4157,11 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0">
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:srgbClr val="434343"/>
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Not Started</a:t>
+            <a:t>Action Req.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4227,10 +4183,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;4:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6466" name="0-4">
+        <xdr:cNvPr id="4808" name="0-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4CD479E-4D9F-D348-E7D0-939B58BD1BED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{619590C4-E030-D811-B77A-208B93B75EE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4315,10 +4271,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;4:4&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6467" name="ExpandIcon">
+        <xdr:cNvPr id="4809" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C86401C6-A3B3-B4DB-F193-E0F9B81F7981}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4033BB65-51A9-1EE4-86BE-94CB6AC60DBA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4359,10 +4315,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6468" name="1-4">
+        <xdr:cNvPr id="4810" name="1-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{608944DD-8179-4D1D-6989-A3834780E6F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{478A5C99-1D9C-599F-DA39-A643CF774F4E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4450,10 +4406,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6469" name="2-4">
+        <xdr:cNvPr id="4811" name="2-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFCB98B8-BE7E-A767-2FBF-9EC7260CB05E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF2CE21C-8863-D886-1978-D6617E683388}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4541,10 +4497,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6470" name="3-4">
+        <xdr:cNvPr id="4812" name="3-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C31F5A0A-0788-D771-3D64-27511A28351B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3CD27E5-B01E-B98C-7C82-BF188EF97F37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4632,10 +4588,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6471" name="4-4">
+        <xdr:cNvPr id="4813" name="4-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2338CAE-E3DD-17FE-B071-E7AA30C5637D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF759AE6-CD25-6119-B707-07C912298341}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4723,10 +4679,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6472" name="5-4">
+        <xdr:cNvPr id="4814" name="5-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B342C5F4-4439-4F57-D53B-E5F81B335B95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F66E623-929E-0B46-A8DC-5F075F193960}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4792,7 +4748,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>1.01</a:t>
+            <a:t>1.12</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4814,10 +4770,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6473" name="6-4">
+        <xdr:cNvPr id="4815" name="6-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5BED6A3-F8F0-BFF5-0872-C442E35166F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098C013A-0BD5-C010-8CD8-6800560A9955}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4883,7 +4839,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fact Find to Client</a:t>
+            <a:t>Chase Emma / Steve</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4905,10 +4861,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6474" name="7-4">
+        <xdr:cNvPr id="4816" name="7-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{385A2F02-5F09-5C68-6E64-B224834010D1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13612BA1-828B-8F0C-8832-F9D0BD09C924}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4925,10 +4881,10 @@
         <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="BAFF29"/>
             </a:gs>
             <a:gs pos="100000">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="BAFF29"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
@@ -4970,11 +4926,11 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0">
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:srgbClr val="434343"/>
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Not Started</a:t>
+            <a:t>Action Req.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4996,10 +4952,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;5:5&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6475" name="0-5">
+        <xdr:cNvPr id="4817" name="0-5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C36AC3F8-5DC0-0A44-9E31-59D33AC03D1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23822AD0-819B-DEAE-A5AA-98466BB8E713}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5084,10 +5040,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;5:5&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6476" name="ExpandIcon">
+        <xdr:cNvPr id="4818" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0096FBE-7647-74F0-4C9E-6934CE167BA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59B03B6C-4FE9-D9E9-26EB-4D741CA60596}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5128,10 +5084,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:5&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6477" name="1-5">
+        <xdr:cNvPr id="4819" name="1-5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6A362E5-5C5F-8DBB-0323-1990B6DD03FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35537781-777D-8E5E-B9B0-0BB5E194EE9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5219,10 +5175,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:5&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6478" name="2-5">
+        <xdr:cNvPr id="4820" name="2-5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95065B05-BCB5-DA07-CD0E-644170844C37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5875B948-F837-029D-4150-A7690392D8DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5310,10 +5266,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:5&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6479" name="3-5">
+        <xdr:cNvPr id="4821" name="3-5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FB58F5C-A128-CB1E-F001-ABE3BB8033AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFC775CE-927F-05A8-3377-58F72B9F2515}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5401,10 +5357,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:5&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6480" name="4-5">
+        <xdr:cNvPr id="4822" name="4-5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CED04F19-92CF-5606-7D5A-EB704DACE06D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63CC1201-F2E2-B86C-E5FD-14450DB966E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5492,10 +5448,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:5&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6481" name="5-5">
+        <xdr:cNvPr id="4823" name="5-5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067BE13F-17AE-23C2-7D16-3DEEE73D63E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FFCC9C0-5668-389C-3420-A2409EBC1401}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5561,7 +5517,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>1.01</a:t>
+            <a:t>1.12</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5583,10 +5539,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:5&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6482" name="6-5">
+        <xdr:cNvPr id="4824" name="6-5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{719E37E9-72B5-561B-22A6-09C73B403815}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DE1047A-3BE7-38BE-2760-6F4805457D44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5652,7 +5608,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fact Find to Client</a:t>
+            <a:t>Chase Emma / Steve</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5674,10 +5630,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:5&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6483" name="7-5">
+        <xdr:cNvPr id="4825" name="7-5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77A406A4-3FE7-0BCF-6801-E51279F76099}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40341958-841C-0B27-8AA9-F03B36E63D2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5694,10 +5650,10 @@
         <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="F1C40F"/>
             </a:gs>
             <a:gs pos="100000">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="F1C40F"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
@@ -5739,11 +5695,11 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0">
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:srgbClr val="434343"/>
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Not Started</a:t>
+            <a:t>Action Req.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5765,10 +5721,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;6:6&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6484" name="0-6">
+        <xdr:cNvPr id="4826" name="0-6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39C2B519-FC73-10C0-340C-7D2C83A74A98}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D59ED4CE-9203-3CF1-4B95-9625E4E05EB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5853,10 +5809,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;6:6&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6485" name="ExpandIcon">
+        <xdr:cNvPr id="4827" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79BB6D68-0DE7-7FEB-448A-E53AACA25B42}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{509B4165-57D7-3869-5E11-0AF78CBDE7E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5897,10 +5853,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:6&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6486" name="1-6">
+        <xdr:cNvPr id="4828" name="1-6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94EBBAEF-3E9C-BFC6-EB98-83FDA5D6C6FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC5380BC-4E50-B26B-A6EE-263FBA9EC6CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5988,10 +5944,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:6&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6487" name="2-6">
+        <xdr:cNvPr id="4830" name="2-6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC8EF800-F4A8-878D-ED85-9C22D621FF87}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5341D85-E170-1215-508B-74D26950E9F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6079,10 +6035,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:6&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6488" name="3-6">
+        <xdr:cNvPr id="4831" name="3-6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{663989E4-362D-2302-DA2A-A9463C41B362}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BFA8521-B6C3-8A4C-29DD-207D98F6E67A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6170,10 +6126,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:6&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6489" name="4-6">
+        <xdr:cNvPr id="4832" name="4-6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{420B6270-9D35-66CF-3DC2-4EE0D1E1BF55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3971484D-3A40-F38A-C92D-B8C365BA2F93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6261,10 +6217,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:6&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6490" name="5-6">
+        <xdr:cNvPr id="4833" name="5-6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38FD79FC-F465-89D3-0BC5-A2C77DCC4469}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{791651C8-7F0D-4607-C192-6B7802509823}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6352,10 +6308,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:6&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6491" name="6-6">
+        <xdr:cNvPr id="4834" name="6-6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7308EB1A-2F33-441D-52EA-89C5950F8780}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8E990DA-6130-AA91-73E6-C9D710E372B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6443,10 +6399,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:6&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6492" name="7-6">
+        <xdr:cNvPr id="4835" name="7-6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E3C08FE-E1A6-D095-992E-DD25D109B020}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5163D66-CB5A-C095-EF1C-94481DDADADA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6534,10 +6490,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;7:8&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6493" name="0-7">
+        <xdr:cNvPr id="4836" name="0-7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD050B78-D82E-0348-74D4-790639FC75C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB3B792B-E84B-9579-E515-47A2FB001100}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6622,10 +6578,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;7:8&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6494" name="ExpandIcon">
+        <xdr:cNvPr id="4837" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0AF7298-020B-16A1-6872-8078AC997B56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9132C98A-C16F-61F7-5CCF-01ADD14BAB7A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6666,10 +6622,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:8&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6495" name="1-7">
+        <xdr:cNvPr id="4838" name="1-7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51C5A7E7-995A-90F8-882F-605CB15E6958}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0E3494-9EB9-3270-3A3A-6823E4EFF7A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6757,10 +6713,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:8&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6496" name="2-7">
+        <xdr:cNvPr id="4839" name="2-7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22D74DB6-642D-3CC5-B3C9-A534A1F5ED19}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20BD51A-8E1E-0733-DFD8-8A0022740444}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6848,10 +6804,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:8&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6497" name="3-7">
+        <xdr:cNvPr id="4840" name="3-7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5F854DC-B259-0A48-859B-0EBCCA99FB24}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E0F98F-EA8B-A0E8-CF8A-784A5E81F4AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6939,10 +6895,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:8&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6498" name="4-7">
+        <xdr:cNvPr id="4841" name="4-7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D09287FE-E90E-5956-F7E0-8167EA128024}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3357333C-D0C0-A2AF-84C8-84546246C9A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7030,10 +6986,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:8&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6499" name="5-7">
+        <xdr:cNvPr id="4842" name="5-7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0693BF34-EDB0-16E6-2C4C-66BE3905D813}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C290E7-29D7-828C-2036-309E6AC06BD4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7099,7 +7055,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>1.01</a:t>
+            <a:t>1.09</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7121,10 +7077,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:8&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6500" name="6-7">
+        <xdr:cNvPr id="4843" name="6-7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D82FFF9D-101A-494E-A14B-574900516538}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6537387E-1DC1-EC1B-7D3A-FA560A9A4693}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7190,7 +7146,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fact Find to Client</a:t>
+            <a:t>Issue Fact Find to Steve / Emma</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7212,10 +7168,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:8&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6501" name="7-7">
+        <xdr:cNvPr id="4844" name="7-7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D12EF668-F68A-3F73-0DA7-D69CDB7C45BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AC4C47D-3D24-453D-BE9A-A37F820AE750}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7232,10 +7188,10 @@
         <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="F1C40F"/>
             </a:gs>
             <a:gs pos="100000">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="F1C40F"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
@@ -7277,11 +7233,11 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0">
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:srgbClr val="434343"/>
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Not Started</a:t>
+            <a:t>Action Req.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7303,10 +7259,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;8:9&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6502" name="0-8">
+        <xdr:cNvPr id="4845" name="0-8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47D97898-D32F-D7E9-D7E5-F9EF38A31949}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3808B4D0-C3C7-D8DA-2BF5-2DBB28AAFD0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7391,10 +7347,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;8:9&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6503" name="ExpandIcon">
+        <xdr:cNvPr id="4846" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BA64A39-1143-AB6A-DC8D-650C2F5EF8CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BB4521D-FD75-E006-B56B-16A27A4CC18D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7435,10 +7391,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:9&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6504" name="1-8">
+        <xdr:cNvPr id="4847" name="1-8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56030139-5FDA-736C-01FE-A683F9EE2775}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{762CE4A4-6AC4-5EE3-8C39-285CFFC11BD4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7526,10 +7482,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:9&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6505" name="2-8">
+        <xdr:cNvPr id="4848" name="2-8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CE7232D-4FD3-D7BD-9A75-AED4ABF9108D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{293B6FD1-300F-2B60-8B0C-11B66ECA90FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7614,10 +7570,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:9&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6506" name="3-8">
+        <xdr:cNvPr id="4849" name="3-8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42026719-7CED-E64E-0FC6-63E49578D720}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32F1A675-3B2B-4E71-1087-6EDD8B2BF072}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7702,10 +7658,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:9&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6507" name="4-8">
+        <xdr:cNvPr id="4850" name="4-8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3068EE4-7FDC-D2C4-A2E2-85BCA5ED336F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FF03F24-2A9F-4F43-606C-6C57FD94C383}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7793,10 +7749,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:9&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6508" name="5-8">
+        <xdr:cNvPr id="4851" name="5-8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51426C4B-AA69-86B5-1458-021C92E998BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF52D270-21FC-7F59-3DBE-98369434D617}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7884,10 +7840,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:9&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6509" name="6-8">
+        <xdr:cNvPr id="4852" name="6-8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6388C3A9-D10E-FC7E-6311-9F07DF9892BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6359E006-6968-133A-6D00-CAC193389B64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7975,10 +7931,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:9&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6510" name="7-8">
+        <xdr:cNvPr id="4853" name="7-8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{493BBD1E-7D57-699D-3596-D5090655A459}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6154EC8D-4540-D0B6-A3F8-03FA3461804E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8066,10 +8022,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;9:10&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6511" name="0-9">
+        <xdr:cNvPr id="4854" name="0-9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD64F397-5FF0-73E4-E9AE-364462DDA502}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{204BBFDE-19C3-1717-9BFC-4B3CE3AF0582}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8154,10 +8110,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;9:10&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6512" name="ExpandIcon">
+        <xdr:cNvPr id="4855" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F174E3DA-684E-3727-52E3-1D60F9A4AE72}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{705E91FF-1E6A-6FC0-2DDD-EFA176D4B1D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8198,10 +8154,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:10&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6513" name="1-9">
+        <xdr:cNvPr id="4856" name="1-9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AC0C1CB-ABCC-26E8-0A2C-BB5916D01413}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{758353E1-D967-A829-AEE7-E41F607CFADB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8289,10 +8245,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:10&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6514" name="2-9">
+        <xdr:cNvPr id="4857" name="2-9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB82507C-2061-B1E6-945E-4B33058AC6DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D5CF3A-7504-6B45-D840-05EA3B22B4FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8380,10 +8336,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:10&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6515" name="3-9">
+        <xdr:cNvPr id="4858" name="3-9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB502A2A-8B2B-28E7-2C11-00DCD2BE1E27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C50199A-DB1C-C325-3267-9753E634FF52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8471,10 +8427,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:10&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6516" name="4-9">
+        <xdr:cNvPr id="4859" name="4-9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5DF1176-0D91-0850-3105-FA33D364318C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF719367-E4E3-D0BE-10CB-442BFD506F47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8562,10 +8518,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:10&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6517" name="5-9">
+        <xdr:cNvPr id="4860" name="5-9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{396B86E5-7C60-5FF6-9F0F-1522579C7BDA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBC96023-845D-30CE-9280-000CF4852E3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8653,10 +8609,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:10&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6518" name="6-9">
+        <xdr:cNvPr id="4861" name="6-9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BE2268F-9F7E-9714-25B3-F3C9A9FE876A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6969C2E3-CBC2-D6AC-BCE8-2E279D1CCBA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8744,10 +8700,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:10&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6519" name="7-9">
+        <xdr:cNvPr id="4862" name="7-9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED5F326C-0B15-A8C0-CFDB-C94AA77FB7EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1009C0B-6900-B47A-3C24-93EE4FA29195}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8835,10 +8791,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;10:11&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6520" name="0-10">
+        <xdr:cNvPr id="4863" name="0-10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87B1ACF1-9CA5-6C1B-02E2-326340D3BAF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A7634DE-7FE6-C50C-24F3-C4CDB6B01F34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8923,10 +8879,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;10:11&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6521" name="ExpandIcon">
+        <xdr:cNvPr id="4864" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6C0D3B5-F5C0-5557-4EF8-93AA852722C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{358FD660-1649-736B-5884-8503F04A7599}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8967,10 +8923,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:11&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6522" name="1-10">
+        <xdr:cNvPr id="4865" name="1-10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32481168-F7F0-2FC1-5716-8BEF77444692}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FF74ADB-D808-DB45-FCD2-157052B73455}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9058,10 +9014,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:11&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6523" name="2-10">
+        <xdr:cNvPr id="4866" name="2-10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B1C294B-E7EE-A218-3D2F-7CD154400C41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAD2B98B-92CC-073C-1983-2FB570015313}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9149,10 +9105,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:11&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6524" name="3-10">
+        <xdr:cNvPr id="4867" name="3-10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCCA6615-B744-109F-02D3-594E110DC77A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E80442F4-78C6-EF78-B6AE-D5462A9D002C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9240,10 +9196,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:11&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6525" name="4-10">
+        <xdr:cNvPr id="4868" name="4-10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F60480D-E414-CBFD-4715-C92508884B4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A440C97-E4E6-EA60-4F7E-0BAA1CAFDF56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9331,10 +9287,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:11&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6526" name="5-10">
+        <xdr:cNvPr id="4869" name="5-10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AEC464B-D693-3C9F-186E-B5C5BD0CA9F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F95B7BB-66AE-2523-D599-647243C7581B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9422,10 +9378,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:11&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6527" name="6-10">
+        <xdr:cNvPr id="4870" name="6-10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{922891E4-2795-1730-8509-22193AEABB7A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4229A03-F774-3E67-5674-9D1DF77CD23E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9513,10 +9469,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:11&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6528" name="7-10">
+        <xdr:cNvPr id="4871" name="7-10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F01FCE5-3962-CFA6-C391-A2A5FA07A5C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9D39B8C-1B93-A36A-20C7-85B48FD1C223}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9604,10 +9560,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;11:12&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6529" name="0-11">
+        <xdr:cNvPr id="4872" name="0-11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3769CAFF-4BC2-5ACD-0212-50279DB9BDFD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34811CC6-2721-AA78-6084-F6E715824A3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9692,10 +9648,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;11:12&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6530" name="ExpandIcon">
+        <xdr:cNvPr id="4873" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CF9A2C9-FE73-475D-9DD1-83D2B79A0471}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79E0427E-300C-C724-7756-EE60DE227A4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9736,10 +9692,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:12&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6531" name="1-11">
+        <xdr:cNvPr id="4874" name="1-11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1241C5B1-12F6-24E0-1787-34EE7B1D6345}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F7FE314-F71D-84DD-1651-EA8910F73619}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9827,10 +9783,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:12&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6532" name="2-11">
+        <xdr:cNvPr id="4875" name="2-11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADC02BCD-9906-62C8-217A-5FE578119060}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAAE058B-64A5-C2DE-0F5A-102AFEA27627}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9918,10 +9874,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:12&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6533" name="3-11">
+        <xdr:cNvPr id="4876" name="3-11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF5B1127-27BE-430F-0608-7E10C0D09867}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EA1ABF4-6636-51BC-7E7F-908FC2A55114}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10009,10 +9965,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:12&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6534" name="4-11">
+        <xdr:cNvPr id="4877" name="4-11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79CD8AE8-9A0C-ACBA-7358-8BD5404FF8B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D6EEC1A-9E06-5F18-A5F2-976E099C98C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10100,10 +10056,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:12&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6535" name="5-11">
+        <xdr:cNvPr id="4878" name="5-11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B21953D-AC54-2A52-14E6-A81A776720C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4B709BB-ECA6-DCFB-F76B-C72B6085636B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10169,7 +10125,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>1.01</a:t>
+            <a:t>1.05</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10191,10 +10147,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:12&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6536" name="6-11">
+        <xdr:cNvPr id="4879" name="6-11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E6B2CDF-F8EC-4B80-347D-56D2FD68B39C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1719FCEA-9D3E-C1FD-FADD-FDAF704C50FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10260,7 +10216,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Fact Find to Client</a:t>
+            <a:t>Perform Basic Review</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10282,10 +10238,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:12&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6537" name="7-11">
+        <xdr:cNvPr id="4880" name="7-11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{188D1272-728C-C768-D281-ABB14FF252F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9BACF0E-F7ED-DCBB-C79E-699C70CB428F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10302,10 +10258,10 @@
         <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="BAFF29"/>
             </a:gs>
             <a:gs pos="100000">
-              <a:srgbClr val="D7263D"/>
+              <a:srgbClr val="BAFF29"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
@@ -10347,7 +10303,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0">
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:srgbClr val="434343"/>
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
@@ -10373,10 +10329,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;12:13&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6538" name="0-12">
+        <xdr:cNvPr id="4881" name="0-12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BB419BB-9887-AEF2-7544-8201C24B63C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A34485DE-157D-359B-7C03-270793679592}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10461,10 +10417,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;12:13&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6539" name="ExpandIcon">
+        <xdr:cNvPr id="4882" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C8D386-9D42-4B11-497F-F8865F092997}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19C2AE22-092F-65D4-8831-DB17B7B76423}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10505,10 +10461,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:13&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6540" name="1-12">
+        <xdr:cNvPr id="4883" name="1-12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AE7684A-128C-9034-E79A-25C19443E50F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54DF59BC-5C0E-26CB-D9FC-34E77CD5943F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10596,10 +10552,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:13&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6541" name="2-12">
+        <xdr:cNvPr id="4884" name="2-12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99BE8975-F838-4D67-6B42-7E177C58DD1E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33F81860-D816-EC3A-A034-A80E43ABA898}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10687,10 +10643,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:13&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6542" name="3-12">
+        <xdr:cNvPr id="4885" name="3-12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51EB200F-CCC0-5B10-548E-58C132E68A99}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93E654EF-8921-8949-B93F-6B77C92631EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10778,10 +10734,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:13&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6543" name="4-12">
+        <xdr:cNvPr id="4886" name="4-12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AC00E7B-7731-9CD9-4C76-4F5F1AB194E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{576147C7-FA01-E197-3E0C-84A9F7AD969F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10869,10 +10825,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:13&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6544" name="5-12">
+        <xdr:cNvPr id="4887" name="5-12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC1178DC-2AF1-0C25-D8DC-612731CD7B28}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF7B5E67-C2B1-966D-64CE-9FEF81E1E967}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10960,10 +10916,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:13&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6545" name="6-12">
+        <xdr:cNvPr id="4888" name="6-12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E950EB0-1285-0443-414C-7531159D8150}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{675842FA-AC60-9593-DEC7-E7FEBFEA8557}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11051,10 +11007,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:13&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6546" name="7-12">
+        <xdr:cNvPr id="4889" name="7-12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C345054-24C5-CCAA-505B-C8D2F692FF2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87EBE045-ABB9-3959-02A8-DC7927EFB170}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11142,10 +11098,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;13:14&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6547" name="0-13">
+        <xdr:cNvPr id="4890" name="0-13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF32A846-ADEF-DE3B-8BAB-0D1336041F00}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCE88475-A52D-0522-EBDC-3E570F4E72BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11230,10 +11186,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;13:14&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6548" name="ExpandIcon">
+        <xdr:cNvPr id="4891" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C242EB6-DE9F-7EE1-6219-A0BFF207B3B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CD9D826-3B64-8A88-D670-9712241E69F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11274,10 +11230,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:14&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6549" name="1-13">
+        <xdr:cNvPr id="4892" name="1-13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6335B33-2F4D-5FA5-E0E2-AEE053249307}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FAB158F-BB66-EC18-D986-F492818CCB55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11365,10 +11321,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:14&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6550" name="2-13">
+        <xdr:cNvPr id="4893" name="2-13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42C4FCD1-CE4D-933A-7E03-2041D4D25F12}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF6BDE3-7242-49D1-FE63-502FD306293D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11456,10 +11412,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:14&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6551" name="3-13">
+        <xdr:cNvPr id="4894" name="3-13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8160543B-A877-C411-19CA-2415B077D26F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F33A491-EF1A-B2C8-5D14-C8D8E65F5F28}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11547,10 +11503,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:14&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6552" name="4-13">
+        <xdr:cNvPr id="4895" name="4-13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5200263-44FE-69DE-2185-86539696037E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A674C60E-C573-C73C-8FCF-E4DED21D90D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11638,10 +11594,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:14&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6553" name="5-13">
+        <xdr:cNvPr id="4896" name="5-13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1D6DA75-F6A0-8D26-3D67-50CCB303A0C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A862334-01D0-3285-1EE3-97463E18C4C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11729,10 +11685,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:14&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6554" name="6-13">
+        <xdr:cNvPr id="4897" name="6-13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B62CF10F-8BEC-6735-BBC5-1F4A2D951B78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34C012D3-D257-B7EC-92D2-819E5086AC1B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11820,10 +11776,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:14&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6555" name="7-13">
+        <xdr:cNvPr id="4898" name="7-13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD69B903-7DB4-BB28-6A31-929E6112C9AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FE238AC-FDEC-02BD-AF38-EEA20493AF39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11911,10 +11867,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;14:15&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6556" name="0-14">
+        <xdr:cNvPr id="4899" name="0-14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8C28400-EEC2-CACE-BAE2-7C8EB361B9F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC642C2D-8704-A0BF-9AD4-18855EDED000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11999,10 +11955,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;14:15&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6557" name="ExpandIcon">
+        <xdr:cNvPr id="4900" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B527E6E-D5A3-A809-E535-D8FB7C4EF5D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9318980D-B58B-1D14-9B2B-94BB1669E0D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12043,10 +11999,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:15&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6558" name="1-14">
+        <xdr:cNvPr id="4901" name="1-14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E3C93E7-0FD5-3BA7-A22A-4FE53DF80776}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B2CFE7-0B98-008F-BD0D-44CA7791C068}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12134,10 +12090,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:15&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6559" name="2-14">
+        <xdr:cNvPr id="4902" name="2-14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{770A75A5-4BAE-DF94-F6A3-F04FD3382251}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1196996-A504-B345-DC2A-ED721BF6DA3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12225,10 +12181,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:15&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6560" name="3-14">
+        <xdr:cNvPr id="4903" name="3-14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{347E8CDB-D6A9-87A6-F8E5-5D312166CC3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72B94AFB-2296-D5F1-88F1-F3F06A732AAB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12316,10 +12272,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:15&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6561" name="4-14">
+        <xdr:cNvPr id="4904" name="4-14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8151A5B8-D3E6-C72B-FAC2-62551B7DE32E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79F3120A-38C4-7E29-77DC-5E8D19ABF573}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12407,10 +12363,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:15&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6562" name="5-14">
+        <xdr:cNvPr id="4905" name="5-14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F6AC8D1-424D-5B5D-DB20-648B0D587990}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E672E4-C08C-AE7D-664C-1EB8A35A73DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12498,10 +12454,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:15&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6563" name="6-14">
+        <xdr:cNvPr id="4906" name="6-14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88711704-5420-9757-6F7A-1736A13EEF66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F141377A-0A18-0F2F-86AE-28B90D892C63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12589,10 +12545,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:15&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6564" name="7-14">
+        <xdr:cNvPr id="4907" name="7-14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3159BDA3-3B2F-F381-F55E-884C0DFD11C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A08DC89-6FD6-F72F-8E11-516BCECC2202}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12680,10 +12636,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;15:16&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6565" name="0-15">
+        <xdr:cNvPr id="4908" name="0-15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C12BFC03-2F00-B55D-C9FF-2B4D43D06EBE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCDE4FB2-4A66-0B18-DF67-349DDF70475E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12768,10 +12724,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;15:16&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6566" name="ExpandIcon">
+        <xdr:cNvPr id="4909" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12FC68AE-BB7D-6368-3940-95DE735A4E27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E964267-27BF-FEDB-64D3-C7A36DA4B08B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12812,10 +12768,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:16&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6567" name="1-15">
+        <xdr:cNvPr id="4910" name="1-15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99C97767-89D5-90A0-F758-CB1794249719}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA536759-666D-AABE-1E31-90BEE89BA93D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12903,10 +12859,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:16&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6568" name="2-15">
+        <xdr:cNvPr id="4911" name="2-15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A228E6FB-61F3-E224-DE27-E3042E94B1C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3F89007-FF62-CAEA-B544-83052CB325B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12994,10 +12950,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:16&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6569" name="3-15">
+        <xdr:cNvPr id="4912" name="3-15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8143B9-C86E-4A20-E61F-087ACB1C99F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D0A93E2-E260-480B-9F6B-E6F138FC6F4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13085,10 +13041,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:16&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6570" name="4-15">
+        <xdr:cNvPr id="4913" name="4-15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB05698F-9CDE-5022-3970-F064A41F57DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688C3959-C576-A9CC-31D7-FC71D8A3F34B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13176,10 +13132,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:16&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6571" name="5-15">
+        <xdr:cNvPr id="4914" name="5-15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34B9A98B-43E3-A511-6BC8-368FCFFA5771}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D65E800-D5E3-E9BB-26B0-026EF00C8CEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13267,10 +13223,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:16&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6572" name="6-15">
+        <xdr:cNvPr id="4915" name="6-15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADA61F02-C7D7-C79F-3317-C4D43BED0B53}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53276580-D5D5-0F5F-871A-3B27A8543299}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13358,10 +13314,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:16&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6573" name="7-15">
+        <xdr:cNvPr id="4916" name="7-15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E42F527-6050-CBD7-F61E-192B930838DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C561ED92-88C8-964F-9E35-A12B68373D4A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13449,10 +13405,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;16:17&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6574" name="0-16">
+        <xdr:cNvPr id="4917" name="0-16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4BCA1FF-B760-A512-D468-B864CC49A66C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86E5D28C-8CDE-1D15-05A7-E4EFD111EE8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13537,10 +13493,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;16:17&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6575" name="ExpandIcon">
+        <xdr:cNvPr id="4918" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57FF2772-F251-356B-0CA3-E1B81B420F48}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52DADE80-7417-5E02-AA23-FB10C1E5BA35}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13581,10 +13537,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:17&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6576" name="1-16">
+        <xdr:cNvPr id="4919" name="1-16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E714C2-C927-1E3B-E52B-B3F7C7092BC9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8793D58-379E-BFB4-D218-E4CC7983EBB6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13672,10 +13628,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:17&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6577" name="2-16">
+        <xdr:cNvPr id="4920" name="2-16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3542A235-28DF-D47E-64E2-E4053ADB5AB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D9ECAA4-BCAF-49B4-AA1C-C25DD696F76A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13763,10 +13719,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:17&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6578" name="3-16">
+        <xdr:cNvPr id="4921" name="3-16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3EBAC4F-C806-492F-EC26-EB64773C8479}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{908C5924-4091-6700-7CB5-2D24C5D1DA32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13854,10 +13810,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:17&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6579" name="4-16">
+        <xdr:cNvPr id="4922" name="4-16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC14A40A-8D0D-697B-8B20-000E31CBDCB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64DAE09A-0BD9-63A4-0BC0-D60E43D8F5AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13945,10 +13901,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:17&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6580" name="5-16">
+        <xdr:cNvPr id="4923" name="5-16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2821ABE-B17B-D7EF-F6E9-3330D3088383}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A8D7AF8-E23D-FA1A-E227-B59A2A50D152}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14036,10 +13992,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:17&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6581" name="6-16">
+        <xdr:cNvPr id="4924" name="6-16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A14D00-F1C6-CD37-8431-C7163854B531}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{086F2ECC-F9AF-57B6-3313-4E91BA9374F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14127,10 +14083,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:17&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6582" name="7-16">
+        <xdr:cNvPr id="4925" name="7-16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A50E9F1-B298-5B82-0781-E0632587FB86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B94C3B87-8D57-33B9-B51A-48B4C09E1B57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14218,10 +14174,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6426" name="Button Frame" hidden="1">
+        <xdr:cNvPr id="32" name="Button Frame" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BFEF528-E0D9-9430-4788-5FFE6C35E2BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B3DAAC6-E03C-C10D-1503-C136C787B86E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14316,10 +14272,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6425" name="Rectangle 6424" hidden="1">
+        <xdr:cNvPr id="31" name="Rectangle 30" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5AB9090-9E25-847B-4C57-DFCEAF0B1785}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F0A7268-53C4-D54A-00D3-F9093D0297CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14376,10 +14332,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:0:0&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6427" name="BtnMain1">
+        <xdr:cNvPr id="33" name="BtnMain1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF6CBDF-0F51-E178-AAA9-4FCFA13298AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA53CACF-C86F-95C1-F464-1C46C668745C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14468,10 +14424,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:3:0&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6428" name="BtnMain2">
+        <xdr:cNvPr id="34" name="BtnMain2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66609E2E-B75F-D752-7FF3-2010FBFD77B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45EDECD3-C351-9286-5741-95EEA60C5878}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14560,10 +14516,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6238" name="MenuBar">
+        <xdr:cNvPr id="4" name="MenuBar">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7749B806-649E-2918-6CE2-1BEDC3BE6C27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{769B6764-94FA-CD73-C402-86FDD9F3BED1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14649,10 +14605,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6237" name="Rectangle 6236" hidden="1">
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B425D5D0-1FCC-0E05-7576-36BE29E00F73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB973AA6-AF4E-FFD8-9303-AA0226D0017E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14709,10 +14665,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6240" name="Logo">
+        <xdr:cNvPr id="6" name="Logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69CB4358-5E75-32B3-7545-06DECF4519E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDBA7AC3-3526-9782-364E-DB78DC977498}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14753,10 +14709,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6242" name="Menu Btn - 1">
+        <xdr:cNvPr id="8" name="Menu Btn - 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C7012A-AE4C-A59F-F6EA-2B432910546F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9002E3ED-6D70-7CF4-7EF5-061AE8AFFF48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14839,10 +14795,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6243" name="Menu Btn - 2">
+        <xdr:cNvPr id="9" name="Menu Btn - 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20E9B469-A19B-F311-08A0-B02C718C3051}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9854EDD9-8343-1AA7-AF8C-3E8180EDDD65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14915,10 +14871,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6244" name="Menu Btn - 2.1" hidden="1">
+        <xdr:cNvPr id="10" name="Menu Btn - 2.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00457ACB-4956-075A-0EF5-FB66BE5937A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54A9C57C-8292-FB54-51CC-2B1E4626C0C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14991,10 +14947,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6245" name="Menu Btn - 2.2" hidden="1">
+        <xdr:cNvPr id="11" name="Menu Btn - 2.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34E2444A-714E-AD83-CB77-C30C120EFF01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F8C1438-04D2-0712-B6BF-5DB753731239}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15067,10 +15023,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6246" name="Menu Btn - 3">
+        <xdr:cNvPr id="12" name="Menu Btn - 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12C1AE36-1390-DBA6-4577-210018E41CE6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D3FA7A3-F1BB-5510-DE0F-EB6CD4AC691B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15143,10 +15099,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6247" name="Menu Btn - 3.1" hidden="1">
+        <xdr:cNvPr id="13" name="Menu Btn - 3.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B210600-3BB4-B083-6165-0B4E0724284D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C4E3C7-E5E8-3BFA-146F-5B025BF5EFAB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15219,10 +15175,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6248" name="Menu Btn - 3.2" hidden="1">
+        <xdr:cNvPr id="14" name="Menu Btn - 3.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F8F7639-CB98-EF36-7B03-D9CB7F0B8DE7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{420DBAB5-923F-FE29-8C54-C532EEB57583}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15295,10 +15251,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6249" name="Menu Btn - 3.3" hidden="1">
+        <xdr:cNvPr id="15" name="Menu Btn - 3.3" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C526ECC7-39A6-B470-3D4B-4D2AC67D26AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEED97C7-4EF5-7936-F658-9F39D2DD43AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15371,10 +15327,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6250" name="Menu Btn - 3.4" hidden="1">
+        <xdr:cNvPr id="16" name="Menu Btn - 3.4" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{946EB83D-DCF7-375C-E3A0-BF6A3F8C6B0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33D59B85-905F-20CA-90FA-0E7771F72BDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15447,10 +15403,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6251" name="Menu Btn - 3.5" hidden="1">
+        <xdr:cNvPr id="17" name="Menu Btn - 3.5" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2625748C-C9E9-157B-9F6D-EF8AC6539F70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB9995D7-B959-5D1E-1F36-D0C2A6981338}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15523,10 +15479,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6252" name="Menu Btn - 4">
+        <xdr:cNvPr id="18" name="Menu Btn - 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{453BD460-A3BA-AA59-7D89-FEF169E2B7B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17B09BDD-EC22-C919-E080-418F7411B33C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15599,10 +15555,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6253" name="Menu Btn - 5">
+        <xdr:cNvPr id="19" name="Menu Btn - 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5622A10F-4699-9FDB-7A6B-321A0FD28037}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A852AB-3871-D983-643F-02F3E4A0958A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15675,10 +15631,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6254" name="Menu Btn - 6">
+        <xdr:cNvPr id="20" name="Menu Btn - 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF08713A-900B-B282-B632-77686F88557A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{017D1C2F-1C0E-30B1-3E51-F07D0F0D8371}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15751,10 +15707,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6255" name="Menu Btn - 6.1" hidden="1">
+        <xdr:cNvPr id="21" name="Menu Btn - 6.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A745227-651C-1F66-6749-8AA553B64591}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458C5ECF-946A-A2B3-6709-636189A2260F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15827,10 +15783,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6256" name="Menu Btn - 6.2" hidden="1">
+        <xdr:cNvPr id="22" name="Menu Btn - 6.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF6B959D-8EFD-C240-1B1A-FB56F602E90C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{466514D1-24D0-E552-BF79-F20DEAB1A946}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15903,10 +15859,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6257" name="Menu Btn - 6.3" hidden="1">
+        <xdr:cNvPr id="23" name="Menu Btn - 6.3" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78EF5EFD-89D0-2C6A-5CE7-FC0C7C55D354}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEFFDA64-C2E1-119E-F3E9-E684EE4A5E4E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15979,10 +15935,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6258" name="Menu Btn - 6.4" hidden="1">
+        <xdr:cNvPr id="24" name="Menu Btn - 6.4" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACF24880-0F8E-CCA3-08E2-CC4C84B9A470}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C8EEEB7-A0C0-7B56-814C-566A9F6F3B51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16055,10 +16011,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6259" name="Menu Btn - 6.5" hidden="1">
+        <xdr:cNvPr id="25" name="Menu Btn - 6.5" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9C83164-F6FB-AFCB-7EEC-58C58A4CC99F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A841F36-6B54-068E-8884-DEC615A51FF3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16131,10 +16087,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6260" name="Menu Btn - 6.6" hidden="1">
+        <xdr:cNvPr id="26" name="Menu Btn - 6.6" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45BCCAA1-1AB6-68BE-E71A-FEC5C9B639F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A95C9F0F-C390-71E4-AFA8-402DAB6B85B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16207,10 +16163,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6261" name="Menu Btn - 6.7" hidden="1">
+        <xdr:cNvPr id="27" name="Menu Btn - 6.7" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0426370-A28D-862C-8561-17D2328B355A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B7ED02-A69E-4BB4-1335-8B75D9AA9C98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16283,10 +16239,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6262" name="Menu Btn - 7">
+        <xdr:cNvPr id="28" name="Menu Btn - 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09F8D0A7-4EFF-020A-CA20-364E0CC3945B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B80E3ED9-D488-9ACF-795C-95650700DEA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16715,6 +16671,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
fix stepaction too small
</commit_message>
<xml_diff>
--- a/CBS Workflow.xlsx
+++ b/CBS Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CBSWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{847FFFD3-8CD9-4FFA-B9E4-D8C999B4F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3D7B5EC-273F-41B1-AF4A-23C65BC24DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25650" yWindow="3120" windowWidth="25695" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39525" yWindow="1125" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -1436,10 +1436,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5502" name="Main Screen">
+        <xdr:cNvPr id="2" name="Main Screen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{369C83D6-FD24-9231-8342-20B24307048F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FDA58D4-D113-4727-6914-93B5E16C24F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1622,10 +1622,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5507" name="Rectangle 5506">
+        <xdr:cNvPr id="7" name="Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8747608B-1E6C-5305-EFEF-4938C8FE81FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A193765-73AA-F971-281F-D77F509FBB3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1682,54 +1682,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5537" name="ExpandIcon">
+        <xdr:cNvPr id="37" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44D9B300-157F-0A78-A04B-CC35B22F7E0E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:link="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1588" cy="1588"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1588</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1588</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5603" name="ExpandIcon">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B8CC367-CF2C-6E59-26C7-4B142E274C61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D5898F1-2995-69BA-5A6C-528F6B0BEA9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1757,2075 +1713,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5774" name="0-0">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF3DDFF6-E05A-500B-B411-91A16DE53B99}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2794000" y="2603500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Workflow No</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5775" name="1-0">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3689757-1837-BC42-1463-0E4B959CB6DE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4064000" y="2603500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Workflow Type</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5776" name="2-0">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DDDFE60-8DF5-51E7-1007-A072668E2352}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5334000" y="2603500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Lender Name</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5777" name="3-0">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3318393A-3DDF-8D53-376D-C0234A1DC734}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7239000" y="2603500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Step No</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5778" name="4-0">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B7B93F7-BF9B-C53A-39ED-D0AF3B624369}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8509000" y="2603500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Step Name</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5779" name="5-0">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{135CED82-5E2C-9564-E208-3E33ACBB6FF7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10414000" y="2603500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Progress</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5780" name="6-0">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2634ABEC-35D1-51A2-8BE7-05830BDE4CBD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12319000" y="2603500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="2AAF92"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Status</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5781" name="0-1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{198946A2-ECC9-CBF3-B569-B11D57922F15}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2794000" y="2857500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>6</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5782" name="1-1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C3CF5FB-ED58-C0F6-FD7B-9CE84A8AFBF4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4064000" y="2857500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Project</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5783" name="2-1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16986234-887C-7AF7-E090-64A65EB3D575}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5334000" y="2857500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>NatWest</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5784" name="3-1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF76DAD5-9E7A-C809-CBA6-E14B6A719A11}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7239000" y="2857500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>1.01</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5785" name="4-1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AB2222-5FDB-B7EF-31FD-764EA6C308DE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8509000" y="2857500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Fact Find to Client</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5786" name="5-1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9765268-AF70-8DCE-DEA3-46D62FBF7AAF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10414000" y="2857500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>%</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:6&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5787" name="6-1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0A4FB6F-E1CC-1AE8-8C97-400B4B474D61}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12319000" y="2857500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="D7263D"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="D7263D"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Not Started</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:33&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5788" name="0-2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD434879-DD78-9411-2DEB-8D9038C07037}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2794000" y="3111500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>33</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:33&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5789" name="1-2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58EA6421-4761-CA31-BA10-E1D6BF64DAE8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4064000" y="3111500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Equity loan</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:33&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5790" name="2-2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5CBEE85-1F94-F3C1-B326-076977816141}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5334000" y="3111500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>NatWest</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:33&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5791" name="3-2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CE3B4AF-4686-D09F-07BC-320663A97D2D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7239000" y="3111500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>4.09</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:33&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5792" name="4-2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22ED3EBE-1FE2-EC98-03C0-0E24D5948DEA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8509000" y="3111500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Exchange Details</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:33&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5793" name="5-2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4FBA8D6-C040-5B94-ABBC-20F526E60C4B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10414000" y="3111500"/>
-          <a:ext cx="1905000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>%</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:2:33&quot;)'" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5794" name="6-2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77B8BF18-04A8-40F9-27BD-5B89D3EFEF45}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12319000" y="3111500"/>
-          <a:ext cx="1270000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="BAFF29"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="BAFF29"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0">
-              <a:solidFill>
-                <a:srgbClr val="434343"/>
-              </a:solidFill>
-              <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Action Req.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5694" name="Frame 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ECD378D-3FCB-BD8C-8375-852D7B18C196}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2159000" y="3492500"/>
-          <a:ext cx="11430000" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="FFFFFF"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-          <a:tileRect/>
-        </a:gradFill>
-        <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="63500" dist="37357" dir="2700000" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="0" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface=""/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5693" name="Rectangle 5692" hidden="1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC04534-EE9D-7B27-227B-211EA4981C71}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="127000" cy="127000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>330200</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -3834,15 +1721,15 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5596" name="Main Frame">
+        <xdr:cNvPr id="30" name="Main Frame">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB508A9A-F8FA-569B-8ED3-52BDF10DCD5D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F35BD3BF-1157-3149-C13A-CF86480006F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3851,7 +1738,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2159000" y="1143000"/>
-          <a:ext cx="11430000" cy="1333500"/>
+          <a:ext cx="11430000" cy="1587500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3937,10 +1824,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5595" name="Main Frame Header">
+        <xdr:cNvPr id="29" name="Main Frame Header">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{776A0201-AC38-A3A3-FEF8-6718972AD420}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9139DE31-EBD1-4C11-D3B9-B79C736459CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4032,10 +1919,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5731" name="0-0">
+        <xdr:cNvPr id="41" name="0-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74BCC2F4-06C2-3790-EA81-7B1E48B7F251}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CF19958-3EBD-3F5D-D2A8-4C3C5A5EDAE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4123,10 +2010,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5732" name="1-0">
+        <xdr:cNvPr id="42" name="1-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D48DC744-B4D8-756E-B563-7C9C9ED50985}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7162115-DED3-3177-6A02-193FF6BAE946}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4214,10 +2101,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5733" name="2-0">
+        <xdr:cNvPr id="43" name="2-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0157853E-CE3D-5E27-3E45-B2DA6EF3742B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{259246BD-2FEF-E0B6-21AC-11F10C852291}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4305,10 +2192,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5734" name="3-0">
+        <xdr:cNvPr id="44" name="3-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E432371-E257-0416-C529-3C1C4EEDB28B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8960907-2A89-71E6-97C7-FCF5010FA2D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4396,10 +2283,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5735" name="4-0">
+        <xdr:cNvPr id="45" name="4-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{549BC901-BC4A-03D1-7542-6CC3983F86C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D9ECB5A-C079-A9E5-4F6E-D6FAABC271C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4487,10 +2374,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5736" name="5-0">
+        <xdr:cNvPr id="46" name="5-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D64E638-EBC1-8C07-7E61-7E72F871B456}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{675FBA57-A656-ED67-01F8-D9576C208883}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4578,10 +2465,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5737" name="6-0">
+        <xdr:cNvPr id="47" name="6-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE20577B-3B10-ABD5-0544-4025BA4161CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D96E4BE-28F8-77BB-A047-78D823155282}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4669,10 +2556,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5738" name="7-0">
+        <xdr:cNvPr id="48" name="7-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3613C983-9817-2524-1392-E83D9A3A0AFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B338801-FDCD-FCFF-E1E1-E69DDAFDFD27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4760,10 +2647,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5739" name="8-0">
+        <xdr:cNvPr id="49" name="8-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C19D93F8-82EE-488E-A0B2-15E4D7243400}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE8172C8-2721-B4BE-DF47-73410194F737}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4851,10 +2738,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5740" name="9-0">
+        <xdr:cNvPr id="50" name="9-0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BCA4B73-F5A5-A530-79CA-1EC8ACA68464}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E55F9C-E3F0-6B7B-BDA0-CD322E914814}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4942,10 +2829,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5741" name="0-1">
+        <xdr:cNvPr id="51" name="0-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6605124E-2915-C0EA-4020-F9D70DD616F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C93C81-E73C-C362-8C1C-6DA88AAFCE37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5030,10 +2917,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;1:1&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5742" name="ExpandIcon">
+        <xdr:cNvPr id="52" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51DE227A-A482-0023-D0E6-CA3C3D6F172E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{578B4CE7-68C7-45AB-3199-E86A5DF88A7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5074,10 +2961,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5743" name="1-1">
+        <xdr:cNvPr id="53" name="1-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67B16596-FB6C-18F8-BEB2-F7E5A0D8A7D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D137B367-A2FF-B2C7-74D0-37354A865CEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5165,10 +3052,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5744" name="2-1">
+        <xdr:cNvPr id="54" name="2-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1899AAAA-5AE4-2149-C729-9E285798245A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E207E2E5-7186-A654-42F6-CFCC6CE8B6AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5256,10 +3143,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5745" name="3-1">
+        <xdr:cNvPr id="55" name="3-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC0F67A-9F1B-5C3E-C445-90ECB8B97031}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3727D53A-7BB0-E913-6B78-61178A7B7DAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5347,10 +3234,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5746" name="4-1">
+        <xdr:cNvPr id="56" name="4-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{974ED045-82ED-6279-647C-CBC8E16C3C7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91AB1CF6-B3D9-E88D-05F5-F347EB7518EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5438,10 +3325,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5747" name="5-1">
+        <xdr:cNvPr id="57" name="5-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90768F26-C433-4CF6-55DD-D73B75F4AC07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93501650-C4EB-0A7A-3D4A-03EDEEBD900E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5529,10 +3416,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5748" name="6-1">
+        <xdr:cNvPr id="58" name="6-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA099CF8-9AE0-CDBB-2F0B-D0E5E44E7382}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CC7B036-A6A8-3F34-B0AF-F992C07DA8B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5620,10 +3507,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5749" name="7-1">
+        <xdr:cNvPr id="59" name="7-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8E30D53-3D01-DBD3-0D98-DD99AD8916CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BD0626-873D-138D-3854-3AB1323ACE9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5711,10 +3598,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5750" name="8-1">
+        <xdr:cNvPr id="60" name="8-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A68555C-8550-D499-F180-AE304411F012}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F61640A1-55E4-AA88-F8B0-A7F2D4A850D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5802,10 +3689,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:1&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5751" name="9-1">
+        <xdr:cNvPr id="61" name="9-1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA19E5B-6C6D-3115-07B7-4A9FE13B06E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3E627B0-104E-BBAD-A211-6C529A4D22EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5893,10 +3780,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;2:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5752" name="0-2">
+        <xdr:cNvPr id="62" name="0-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3EADD94-9AE0-2EF8-9D5E-1D3F5A9E5367}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F4F1C98-A8F2-00A0-3AD1-725747716546}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5981,10 +3868,10 @@
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;2:2&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5753" name="ExpandIcon">
+        <xdr:cNvPr id="63" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5A7EFE2-89E5-549F-EB9E-4631511B4B1F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B5A88F7-B395-949A-287E-7ECF1100BB57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6025,10 +3912,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5754" name="1-2">
+        <xdr:cNvPr id="4800" name="1-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59AB8DEF-2C39-DFC9-09EA-7CFAFBA12979}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1386E28C-C879-1F54-BFA2-BD71913928B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6116,10 +4003,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5755" name="2-2">
+        <xdr:cNvPr id="4801" name="2-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8448868C-C922-DA50-7315-CA66986FBD28}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70B7FDFB-3E68-BAC7-DBA1-9CD91B3C4F81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6207,10 +4094,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5756" name="3-2">
+        <xdr:cNvPr id="4802" name="3-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCF9D7B8-16BF-4444-54C4-2154EA85C972}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5685E704-E2FB-E79E-4ECF-B591AD207D30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6298,10 +4185,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5757" name="4-2">
+        <xdr:cNvPr id="4803" name="4-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60897899-E393-4C2B-B5FE-7635299DB492}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{291D3E76-DF46-5EC6-5128-99274177EBF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6389,10 +4276,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5758" name="5-2">
+        <xdr:cNvPr id="4804" name="5-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14097CDB-798B-552B-9A36-D44102ACBE38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6004F277-C9CC-1EB9-B602-28AFA553A5BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6480,10 +4367,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5759" name="6-2">
+        <xdr:cNvPr id="4805" name="6-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3E23309-0342-D7A1-A0F3-BE0441848DD4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8D365CC-55BF-A5E1-D9DD-56DEF979CCCA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6571,10 +4458,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5760" name="7-2">
+        <xdr:cNvPr id="4806" name="7-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EDA9412-F0D5-9D69-64D3-80484260F1E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{260A0827-F3D4-F387-4E2B-C9A9905EBD3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6662,10 +4549,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5761" name="8-2">
+        <xdr:cNvPr id="4807" name="8-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA2029BF-250C-5AB6-BA11-20CEACF8E566}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FE2EEE5-04C7-6226-886A-F266E49A6B1B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6753,10 +4640,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:2&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5762" name="9-2">
+        <xdr:cNvPr id="4808" name="9-2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B2E6F51-A433-2BCA-B637-5B62A2487158}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4F1802B-E517-E46F-DCCA-5A2C8A6DF9AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6844,10 +4731,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;3:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5763" name="0-3">
+        <xdr:cNvPr id="4809" name="0-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07B5BCD7-F181-1D88-D185-FBC4202A7C2D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3182263C-7225-A3D3-56CE-6E4471CA6170}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6920,22 +4807,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>547688</xdr:colOff>
+      <xdr:colOff>584200</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>103188</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;3:3&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5764" name="ExpandIcon">
+        <xdr:cNvPr id="4810" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D42C35-61A2-B32F-451A-FC927C17C1FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D01F744-0302-A102-C383-C4D011A0F687}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6950,8 +4837,8 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="2389188" y="2247900"/>
+        <a:xfrm>
+          <a:off x="2413000" y="2260600"/>
           <a:ext cx="139700" cy="165100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6976,10 +4863,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5765" name="1-3">
+        <xdr:cNvPr id="4811" name="1-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BADC55A5-FD3F-447C-8EB4-E76EE91FB832}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1707443-2A30-A11B-0B44-3C36A59DCE4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7067,10 +4954,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5766" name="2-3">
+        <xdr:cNvPr id="4812" name="2-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E969D9EB-9F18-E017-5283-9CB3CA990392}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B45136D-2FE9-58B7-FC9A-1A4DA94387BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7158,10 +5045,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5767" name="3-3">
+        <xdr:cNvPr id="4813" name="3-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CA51D51-FA32-79BF-9421-B7C0990EEA77}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B45D2F5C-E6A8-27A8-0653-C2382D20A72A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7249,10 +5136,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5768" name="4-3">
+        <xdr:cNvPr id="4814" name="4-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5E2F72A-9FF4-2E32-6466-D13095B88BB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E08E8C7-2D8D-72DD-D1D5-1521616A8CAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7340,10 +5227,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5769" name="5-3">
+        <xdr:cNvPr id="4815" name="5-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61CF7DA7-09C1-8B08-4356-75F86BBDC20D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC54FB9-18D4-C2D8-D8DE-C647B2FD1BA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7431,10 +5318,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5770" name="6-3">
+        <xdr:cNvPr id="4816" name="6-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86171D66-C4C6-C318-E372-FFF25DF69FCE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71603BB6-B42F-4E05-95D3-16AF42696199}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7522,10 +5409,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5771" name="7-3">
+        <xdr:cNvPr id="4817" name="7-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A9F9B05-5B34-3DAF-CBBB-AE5E6893A560}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A9844C2-3C84-4E6B-5F54-B4B014103223}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7613,10 +5500,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5772" name="8-3">
+        <xdr:cNvPr id="4818" name="8-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45F0DAB-78B9-0388-A7CA-319E7FD81B20}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F75A4C1-E0FE-53FE-700B-C8345D09B3EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7704,10 +5591,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:3&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5773" name="9-3">
+        <xdr:cNvPr id="4819" name="9-3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85CD570B-DAC7-E81D-9D87-6DD05CB7CC66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF4E7AFB-DAFA-398B-7668-3B46FB5471C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7784,21 +5671,21 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIProjects.SplitScreen(&quot;4:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5795" name="0-4">
+        <xdr:cNvPr id="4820" name="0-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A19A4F23-5C26-FE58-AAF0-2883931B1AEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0391ADFA-84BB-A95D-4201-9F0EE67930C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7806,7 +5693,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2159000" y="3492500"/>
+          <a:off x="2159000" y="2476500"/>
           <a:ext cx="635000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7872,21 +5759,21 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="'ModUIProjects.SplitScreen(&quot;4:4&quot;)'">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5796" name="ExpandIcon">
+        <xdr:cNvPr id="4821" name="ExpandIcon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AC52F59-1778-6799-413B-28783BC87732}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5350DE8-F37A-0A84-C8E5-B094C486EF30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7902,7 +5789,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2413000" y="3530600"/>
+          <a:off x="2413000" y="2514600"/>
           <a:ext cx="139700" cy="165100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7916,21 +5803,21 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5797" name="1-4">
+        <xdr:cNvPr id="4822" name="1-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AA6C8A6-8E2F-DAE2-9EB1-AD12EF057679}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAD674E9-49B8-C75C-F306-F3881D0775A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7938,7 +5825,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2794000" y="3492500"/>
+          <a:off x="2794000" y="2476500"/>
           <a:ext cx="635000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8007,21 +5894,21 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5798" name="2-4">
+        <xdr:cNvPr id="4823" name="2-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08261B97-2A12-D28B-150D-444115B91FDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70DBBE44-002F-6E79-E978-B5633F834693}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8029,7 +5916,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3429000" y="3492500"/>
+          <a:off x="3429000" y="2476500"/>
           <a:ext cx="1270000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8098,21 +5985,21 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5799" name="3-4">
+        <xdr:cNvPr id="4824" name="3-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D7040B1-2CE2-59DF-E216-D9AC127C9A36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF064A4-DE7D-AA0E-E1F5-223C833BB6BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8120,7 +6007,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4699000" y="3492500"/>
+          <a:off x="4699000" y="2476500"/>
           <a:ext cx="1270000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8189,21 +6076,21 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5800" name="4-4">
+        <xdr:cNvPr id="4825" name="4-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{977CB3EA-E727-E98E-6BAE-688B7C0ABFEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB2D1F90-F96C-599D-4226-1AA65CED4263}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8211,7 +6098,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5969000" y="3492500"/>
+          <a:off x="5969000" y="2476500"/>
           <a:ext cx="1270000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8280,21 +6167,21 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5801" name="5-4">
+        <xdr:cNvPr id="4826" name="5-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82B0E288-1121-0678-3F7F-06E349165849}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B09F3418-4185-094A-FCE3-AEFCC2941667}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8302,7 +6189,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7239000" y="3492500"/>
+          <a:off x="7239000" y="2476500"/>
           <a:ext cx="1270000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8371,21 +6258,21 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5802" name="6-4">
+        <xdr:cNvPr id="4827" name="6-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E138DE28-665B-4025-8A37-E01261FC4F85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A94BCF62-EAA9-EECB-FBB7-E2F4B8101182}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8393,7 +6280,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8509000" y="3492500"/>
+          <a:off x="8509000" y="2476500"/>
           <a:ext cx="635000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8462,21 +6349,21 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5803" name="7-4">
+        <xdr:cNvPr id="4828" name="7-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46B9F1DB-5007-AC6A-CD09-FCE60B8274FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B708715B-A432-0F69-63DA-C84AD79B2EA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8484,7 +6371,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9144000" y="3492500"/>
+          <a:off x="9144000" y="2476500"/>
           <a:ext cx="1905000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8553,21 +6440,21 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5804" name="8-4">
+        <xdr:cNvPr id="4830" name="8-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5CC99A1-9CCB-645A-5A52-6DA5BA84095D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12AEB46B-8D06-7920-10BF-A46898A4B081}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8575,7 +6462,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11049000" y="3492500"/>
+          <a:off x="11049000" y="2476500"/>
           <a:ext cx="1270000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8644,21 +6531,21 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:1:4&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5805" name="9-4">
+        <xdr:cNvPr id="4831" name="9-4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C090BE98-F9F4-4591-D329-43978F2E7D38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCC39345-D3A5-6BA5-C25D-143CCE199290}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8666,7 +6553,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12319000" y="3492500"/>
+          <a:off x="12319000" y="2476500"/>
           <a:ext cx="1270000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8675,10 +6562,10 @@
         <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
-              <a:srgbClr val="F1C40F"/>
+              <a:srgbClr val="D7263D"/>
             </a:gs>
             <a:gs pos="100000">
-              <a:srgbClr val="F1C40F"/>
+              <a:srgbClr val="D7263D"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="1"/>
@@ -8720,7 +6607,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0">
               <a:solidFill>
-                <a:srgbClr val="434343"/>
+                <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
@@ -8746,10 +6633,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5598" name="Button Frame" hidden="1">
+        <xdr:cNvPr id="32" name="Button Frame" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C17370F-10DC-EEE9-4F3D-AB57C6F5C69D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{123385FE-4C71-FE06-485F-BD38D49B9066}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8844,10 +6731,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5597" name="Rectangle 5596" hidden="1">
+        <xdr:cNvPr id="31" name="Rectangle 30" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{562EB26D-D1FB-19C7-F17B-8C56637912C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{092A7F5B-C52A-A35F-1A92-52301B715B99}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8904,10 +6791,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:0:0&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5600" name="BtnMain1">
+        <xdr:cNvPr id="34" name="BtnMain1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58D019E0-E282-2915-85A5-0A2EB24974BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97ED0ACA-2B1C-3368-7014-D41D25AF6579}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8996,10 +6883,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:3:0&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5601" name="BtnMain2">
+        <xdr:cNvPr id="35" name="BtnMain2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C07C352-9774-347D-0B0B-C604B399EBE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88AB3A2B-49B5-94AF-8711-4490310C1E6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9088,10 +6975,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIButtonHandler.ProcessBtnClicks(&quot;0:10:0&quot;)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5599" name="BtnMain3">
+        <xdr:cNvPr id="33" name="BtnMain3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEFF9813-C259-23D9-BBAF-AB410C0487B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50ED728B-1FCE-9146-8011-EDE042CA345C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9180,10 +7067,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5605" name="ToDo Icon">
+        <xdr:cNvPr id="39" name="ToDo Icon">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00FDF580-5C5B-548B-A5ED-FB0A0B0CBEC6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C5E8518-8410-E028-2CE5-5F28E4E2BC0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9224,10 +7111,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5606" name="ToDo Badge">
+        <xdr:cNvPr id="40" name="ToDo Badge">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C05DAD3A-40EE-D35D-F282-DA3364F83B31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{616D83E2-0F41-974A-CEC2-7B53A1E9EFC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9285,7 +7172,7 @@
               </a:solidFill>
               <a:latin typeface="Eras Medium ITC" panose="020B0602030504020804" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>0</a:t>
+            <a:t>1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -9307,10 +7194,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5504" name="MenuBar">
+        <xdr:cNvPr id="4" name="MenuBar">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3878B7E-737A-4315-100D-577D26538F94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D55F67-CE8C-BB19-FE6E-89012BDCAD23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9396,10 +7283,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5503" name="Rectangle 5502" hidden="1">
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCFFA8FD-167F-97ED-CCEA-6572624E0E68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E03F3C17-C20F-FA35-42D1-5DF37C5DBC11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9456,10 +7343,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5506" name="Logo">
+        <xdr:cNvPr id="6" name="Logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA3DA9E2-399A-5732-4AEB-A19A589D9C8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7555989B-DFC3-6106-66A0-CEAA8A275457}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9500,10 +7387,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5508" name="Menu Btn - 1">
+        <xdr:cNvPr id="8" name="Menu Btn - 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C10D07B-F76C-A73C-A629-29CEFD2D6775}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F362E0B-39C8-BC7E-1AB8-AC590F57E11F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9586,10 +7473,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5509" name="Menu Btn - 2">
+        <xdr:cNvPr id="9" name="Menu Btn - 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A943CB2A-95BE-F859-547A-4E4BD0F8CBA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9B8FDB3-BD32-EFFD-3067-A8AF112F50D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9662,10 +7549,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5510" name="Menu Btn - 2.1" hidden="1">
+        <xdr:cNvPr id="10" name="Menu Btn - 2.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D494396E-D2F9-09C0-9674-4163133D608B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8039404-9F22-A5A2-D4C1-6ED86A9CC973}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9738,10 +7625,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(2.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5511" name="Menu Btn - 2.2" hidden="1">
+        <xdr:cNvPr id="11" name="Menu Btn - 2.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22FDB6F8-E9BB-05B9-369C-61F102EBF8B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9ACAA5F-AF74-FA3D-481A-0F6E852BDEEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9814,10 +7701,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5512" name="Menu Btn - 3">
+        <xdr:cNvPr id="12" name="Menu Btn - 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{725B17A2-DF3A-9C91-2514-BA479E1A90FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF2F2E4B-BFA9-5924-7235-69368F9F2FF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9890,10 +7777,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5513" name="Menu Btn - 3.1" hidden="1">
+        <xdr:cNvPr id="13" name="Menu Btn - 3.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2810A296-470A-01AA-6E63-751DA794C689}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4571C063-6137-BD52-DF72-5BBA16489CF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9966,10 +7853,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5514" name="Menu Btn - 3.2" hidden="1">
+        <xdr:cNvPr id="14" name="Menu Btn - 3.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{728B681B-8D96-0F65-1699-32AEE780D0D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2697AC45-3584-CA4A-8C53-2F1F0A3C7D5F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10042,10 +7929,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5515" name="Menu Btn - 3.3" hidden="1">
+        <xdr:cNvPr id="15" name="Menu Btn - 3.3" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8A28028-A1D4-415E-4927-E230642A350D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4108729A-04F6-3E7A-F0B5-F52E17EA0BCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10118,10 +8005,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5516" name="Menu Btn - 3.4" hidden="1">
+        <xdr:cNvPr id="16" name="Menu Btn - 3.4" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00EC4AD0-7D56-8580-E1C1-057E7DC5A752}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C1D8D5A-A932-1B1C-727B-0E216A598B8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10194,10 +8081,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(3.5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5517" name="Menu Btn - 3.5" hidden="1">
+        <xdr:cNvPr id="17" name="Menu Btn - 3.5" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E15950D5-9DCC-AC47-118C-F697A3F8AECA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18B7566C-11AC-1A52-C5E7-01F74AFC4130}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10270,10 +8157,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5518" name="Menu Btn - 4">
+        <xdr:cNvPr id="18" name="Menu Btn - 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F31B5D95-A683-0CF2-BA06-392D31C556D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84449AE3-9437-565E-986F-D04523470D66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10346,10 +8233,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5519" name="Menu Btn - 5">
+        <xdr:cNvPr id="19" name="Menu Btn - 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62DD55F0-0C00-A5C8-7E85-1BA773D5AD37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AE9B5DC-36C1-7CDD-0EB6-9D7E56447926}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10422,10 +8309,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5520" name="Menu Btn - 6">
+        <xdr:cNvPr id="20" name="Menu Btn - 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{975BB7F8-8223-D149-4C6C-0A4E7DD7C5D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C56E72-E052-B557-48C4-1AE4F1D1FFD1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10498,10 +8385,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.1)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5521" name="Menu Btn - 6.1" hidden="1">
+        <xdr:cNvPr id="21" name="Menu Btn - 6.1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10ABEEE5-C256-088D-C496-6979F1B93A9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ED96553-7754-3AA9-43F1-1D4FE5199FE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10574,10 +8461,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.2)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5522" name="Menu Btn - 6.2" hidden="1">
+        <xdr:cNvPr id="22" name="Menu Btn - 6.2" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{756BCD2B-9BD0-DF57-F9FA-D6A9299893A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38DADFA1-C869-FA38-8E4D-55D1215F0FC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10650,10 +8537,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.3)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5523" name="Menu Btn - 6.3" hidden="1">
+        <xdr:cNvPr id="23" name="Menu Btn - 6.3" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28310A08-72C2-5816-FC09-200666647AF9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6171A2EB-6628-183A-64B1-1FC517432E69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10726,10 +8613,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.4)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5524" name="Menu Btn - 6.4" hidden="1">
+        <xdr:cNvPr id="24" name="Menu Btn - 6.4" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C0FDB1E-3EC2-2070-71F6-03D27052B9E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEC67948-B80C-1CF7-E7C0-DCDF276DB16B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10802,10 +8689,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.5)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5525" name="Menu Btn - 6.5" hidden="1">
+        <xdr:cNvPr id="25" name="Menu Btn - 6.5" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E43B4184-CE6A-A9D5-5B34-B85FC6AB491A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2087197A-5CDD-95E8-9B35-D3B4DCBDE053}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10878,10 +8765,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.6)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5526" name="Menu Btn - 6.6" hidden="1">
+        <xdr:cNvPr id="26" name="Menu Btn - 6.6" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C2E6CD5-0165-5984-F696-41C70A908738}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B1971CB-9C4D-5377-E057-2147BAE9D7D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10954,10 +8841,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(6.7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5527" name="Menu Btn - 6.7" hidden="1">
+        <xdr:cNvPr id="27" name="Menu Btn - 6.7" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA645087-5644-6CCC-8871-63E45B04F2DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38834357-2EE9-ED9A-BC5A-EA795452B81C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11030,10 +8917,10 @@
     </xdr:to>
     <xdr:sp macro="'ModUIMenu.ButtonClickEvent(7)'" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5528" name="Menu Btn - 7">
+        <xdr:cNvPr id="28" name="Menu Btn - 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BC46F1A-D1F5-8514-6A34-B516B564B1A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{553FF493-F063-0BA1-16B6-F0ABF726968C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>